<commit_message>
Added untested code to ballhandler, fixed controls
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -421,6 +421,15 @@
   </si>
   <si>
     <t>Kilroy Equipment List (2022)</t>
+  </si>
+  <si>
+    <t>Left Operator Intake</t>
+  </si>
+  <si>
+    <t>operatorIntakeButtonPressed</t>
+  </si>
+  <si>
+    <t>Left Operator Trigger</t>
   </si>
 </sst>
 </file>
@@ -798,11 +807,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1113,7 +1122,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1124,8 +1133,8 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1142,13 +1151,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
@@ -1170,10 +1179,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1464,10 +1473,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="69" t="s">
+      <c r="C28" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="69"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="9" t="s">
         <v>20</v>
       </c>
@@ -1599,10 +1608,10 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="69" t="s">
+      <c r="C45" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="69"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="9" t="s">
         <v>28</v>
       </c>
@@ -1646,10 +1655,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="69" t="s">
+      <c r="C50" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="69"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="9" t="s">
         <v>31</v>
       </c>
@@ -1705,10 +1714,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="38"/>
-      <c r="C57" s="69" t="s">
+      <c r="C57" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="D57" s="69"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="9" t="s">
         <v>35</v>
       </c>
@@ -1750,10 +1759,10 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="69" t="s">
+      <c r="C62" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="D62" s="69"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="9" t="s">
         <v>39</v>
       </c>
@@ -1798,10 +1807,10 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
-      <c r="C68" s="69" t="s">
+      <c r="C68" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D68" s="69"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="9" t="s">
         <v>41</v>
       </c>
@@ -1845,10 +1854,10 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="38"/>
-      <c r="C73" s="69" t="s">
+      <c r="C73" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="D73" s="69"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="9" t="s">
         <v>45</v>
       </c>
@@ -1913,10 +1922,10 @@
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="38"/>
-      <c r="C78" s="69" t="s">
+      <c r="C78" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="D78" s="69"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="9" t="s">
         <v>58</v>
       </c>
@@ -1974,12 +1983,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="43"/>
       <c r="B83" s="43"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="13"/>
+      <c r="C83" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D83" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E83" s="66" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="22"/>
@@ -2096,10 +2111,10 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
-      <c r="C99" s="69" t="s">
+      <c r="C99" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="D99" s="69"/>
+      <c r="D99" s="70"/>
       <c r="E99" s="9" t="s">
         <v>58</v>
       </c>
@@ -3177,11 +3192,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3189,6 +3199,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Worked on an commented launcher
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -48,27 +48,15 @@
     <t>Left Front Motor (controller_type)</t>
   </si>
   <si>
-    <t>leftFrontMotor</t>
-  </si>
-  <si>
     <t>Right Front Motor (controller_type)</t>
   </si>
   <si>
-    <t>rightFrontMotor</t>
-  </si>
-  <si>
     <t>Left Rear Motor (controller_type)</t>
   </si>
   <si>
-    <t>leftRearMotor</t>
-  </si>
-  <si>
     <t>Right Rear Motor (controller_type)</t>
   </si>
   <si>
-    <t>rightRearMotor</t>
-  </si>
-  <si>
     <t>Left Drive Encoder</t>
   </si>
   <si>
@@ -264,9 +252,6 @@
     <t>Transmission</t>
   </si>
   <si>
-    <t>transmission</t>
-  </si>
-  <si>
     <t>Kilroy-Laptops</t>
   </si>
   <si>
@@ -357,12 +342,6 @@
     <t>Left Drivers Gear Up</t>
   </si>
   <si>
-    <t>rightDriverCameraSwitchButtonPressed</t>
-  </si>
-  <si>
-    <t>rightOperatorCameraSwitchButtonPressed</t>
-  </si>
-  <si>
     <t>CAN 12</t>
   </si>
   <si>
@@ -430,6 +409,153 @@
   </si>
   <si>
     <t>Left Operator Trigger</t>
+  </si>
+  <si>
+    <t>leftTopMotor</t>
+  </si>
+  <si>
+    <t>rightTopMotor</t>
+  </si>
+  <si>
+    <t>leftBottomMotor</t>
+  </si>
+  <si>
+    <t>rightBottomMotor</t>
+  </si>
+  <si>
+    <t>ballCountInitSwitch</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>spinSwitch</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>floorLight</t>
+  </si>
+  <si>
+    <t>Spin Switch</t>
+  </si>
+  <si>
+    <t>Ball Counter Switch</t>
+  </si>
+  <si>
+    <t>intakePiston</t>
+  </si>
+  <si>
+    <t>Intake Piston</t>
+  </si>
+  <si>
+    <t>rightOperatorCameraSwitchButton</t>
+  </si>
+  <si>
+    <t>rightDriverCameraSwitchButton</t>
+  </si>
+  <si>
+    <t>launchButton</t>
+  </si>
+  <si>
+    <t>launchDisableButton</t>
+  </si>
+  <si>
+    <t>subtractBallButton</t>
+  </si>
+  <si>
+    <t>addBallButton</t>
+  </si>
+  <si>
+    <t>Right 5</t>
+  </si>
+  <si>
+    <t>Right1</t>
+  </si>
+  <si>
+    <t>Right 9</t>
+  </si>
+  <si>
+    <t>Right 8</t>
+  </si>
+  <si>
+    <t>Launch Ball</t>
+  </si>
+  <si>
+    <t>Disable Launch</t>
+  </si>
+  <si>
+    <t>Subtract from Ball Count</t>
+  </si>
+  <si>
+    <t>Add to Ball Count</t>
+  </si>
+  <si>
+    <t>Floor Light</t>
+  </si>
+  <si>
+    <t>launchMotorForward</t>
+  </si>
+  <si>
+    <t>launchMotorBackward</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Intake Motor</t>
+  </si>
+  <si>
+    <t>intakeMotor</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Launch Motor Forward</t>
+  </si>
+  <si>
+    <t>Launch Motor Backward</t>
+  </si>
+  <si>
+    <t>colorWheelMotor</t>
+  </si>
+  <si>
+    <t>Color Wheel Motor</t>
+  </si>
+  <si>
+    <t>5, 4</t>
+  </si>
+  <si>
+    <t>launcher</t>
+  </si>
+  <si>
+    <t>Launcher</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor</t>
+  </si>
+  <si>
+    <t>ultraSonic</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>compressor</t>
+  </si>
+  <si>
+    <t>tankTransmission</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>PCB</t>
   </si>
 </sst>
 </file>
@@ -636,36 +762,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -807,14 +930,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1122,7 +1248,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1132,34 +1258,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="69" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1179,10 +1305,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1193,1126 +1319,1216 @@
       <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19" t="s">
+      <c r="D7" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D10" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="23" customFormat="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D11" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="64" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="65" t="s">
+      <c r="C12" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+      <c r="E12" s="65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="64"/>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="C14" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="71" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="70"/>
+      <c r="E19" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="68"/>
+      <c r="E28" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="64" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="66" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="66" t="s">
-        <v>128</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-    </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-    </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-    </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+      <c r="E29" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+      <c r="C30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="C32" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="21"/>
-    </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="21"/>
-    </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="21"/>
-    </row>
-    <row r="41" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="17"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="21"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="20"/>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="70" t="s">
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="68"/>
+      <c r="E45" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A46" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+    </row>
+    <row r="47" spans="1:5" s="4" customFormat="1">
+      <c r="A47" s="49"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="68"/>
+      <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="9" t="s">
+    </row>
+    <row r="51" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="52" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
-      <c r="A46" s="47" t="s">
+      <c r="D51" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-    </row>
-    <row r="47" spans="1:5" s="4" customFormat="1">
-      <c r="A47" s="50"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="31"/>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
-      <c r="A48" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="70" t="s">
+      <c r="E51" s="48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="16"/>
+    </row>
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="9" t="s">
+      <c r="D57" s="68"/>
+      <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="53" t="s">
+    <row r="58" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A58" s="51"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="D58" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E58" s="48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="16"/>
+    </row>
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="68"/>
+      <c r="E62" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A63" s="51"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="16"/>
+    </row>
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="16"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
+    </row>
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="68"/>
+      <c r="E68" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="16"/>
+    </row>
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="16"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+    </row>
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="68"/>
+      <c r="E73" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G73" s="55"/>
+    </row>
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" s="55"/>
+    </row>
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G75" s="55"/>
+    </row>
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A76" s="17"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" s="55"/>
+    </row>
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G77" s="55"/>
+    </row>
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="68" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="13"/>
-    </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="70"/>
-      <c r="E57" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A58" s="52"/>
-      <c r="B58" s="52"/>
-      <c r="C58" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="13"/>
-    </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A62" s="38"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="D62" s="70"/>
-      <c r="E62" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:8" s="54" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="17"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
-    </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A68" s="38"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="42"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="13"/>
-    </row>
-    <row r="72" spans="1:8" s="54" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="17"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55"/>
-    </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A73" s="38"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="D73" s="70"/>
-      <c r="E73" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G73" s="56"/>
-    </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G74" s="56"/>
-    </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G75" s="56"/>
-    </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G76" s="56"/>
-    </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
-      <c r="C77" s="29" t="s">
+      <c r="D78" s="68"/>
+      <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G77" s="56"/>
-    </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A78" s="38"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="70"/>
-      <c r="E78" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G78" s="56"/>
+      <c r="G78" s="55"/>
     </row>
     <row r="79" spans="1:8" s="4" customFormat="1" ht="25.5">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="D79" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E79" s="33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="54" customFormat="1" ht="25.5">
-      <c r="A80" s="22"/>
-      <c r="B80" s="22"/>
-      <c r="C80" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="D80" s="67" t="s">
-        <v>111</v>
-      </c>
-      <c r="E80" s="64" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
-      <c r="A81" s="58"/>
-      <c r="B81" s="58"/>
-      <c r="C81" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
-      <c r="A82" s="22"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="64" t="s">
+      <c r="A79" s="17"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D80" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="E80" s="63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A81" s="57"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D82" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="64" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D83" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="E83" s="66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
-      <c r="A84" s="22"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="17"/>
+      <c r="D81" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E81" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+      <c r="A83" s="42"/>
+      <c r="B83" s="42"/>
+      <c r="C83" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E83" s="65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D84" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E84" s="63" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="85" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A85" s="5"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="56"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
-      <c r="A86" s="22"/>
-      <c r="B86" s="22"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E85" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="F85" s="55"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D86" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="E86" s="63" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
-      <c r="B87" s="18"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="56"/>
-    </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="17"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="D87" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E87" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F87" s="55"/>
+    </row>
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="16"/>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="57"/>
-      <c r="F89" s="56"/>
-    </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
-      <c r="A90" s="22"/>
-      <c r="B90" s="22"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="55"/>
+    </row>
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="16"/>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="56"/>
-    </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
-      <c r="A92" s="22"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="17"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="55"/>
+    </row>
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="16"/>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="56"/>
-    </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="17"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="55"/>
+    </row>
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="16"/>
     </row>
     <row r="95" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A95" s="5"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="31"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="56"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="55"/>
     </row>
     <row r="96" spans="1:6" s="4" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A96" s="22"/>
-      <c r="B96" s="22"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="17"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="16"/>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A97" s="5"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="56"/>
-    </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
-      <c r="A98" s="22"/>
-      <c r="B98" s="22"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="17"/>
-    </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A99" s="38"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="70" t="s">
+      <c r="B97" s="17"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="55"/>
+    </row>
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="16"/>
+    </row>
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D99" s="68"/>
+      <c r="E99" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G99" s="55"/>
+    </row>
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A100" s="17"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E100" s="41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="16"/>
+    </row>
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A102" s="37"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D102" s="59"/>
+      <c r="E102" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D99" s="70"/>
-      <c r="E99" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G99" s="56"/>
-    </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
-      <c r="A100" s="18"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D100" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="E100" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
-      <c r="A101" s="22"/>
-      <c r="B101" s="22"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="17"/>
-    </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
-      <c r="A102" s="38"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D102" s="60"/>
-      <c r="E102" s="39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    </row>
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
-      <c r="C103" s="42"/>
-      <c r="D103" s="34"/>
-      <c r="E103" s="21"/>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
-      <c r="A104" s="22"/>
-      <c r="B104" s="22"/>
-      <c r="C104" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+      <c r="C103" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D103" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="E103" s="65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
-      <c r="C105" s="42" t="s">
+      <c r="C105" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D105" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E105" s="60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D105" s="34" t="s">
+      <c r="E106" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="E105" s="61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D106" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E106" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    </row>
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
-      <c r="C107" s="31"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="21"/>
-    </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
-      <c r="A108" s="22"/>
-      <c r="B108" s="22"/>
-      <c r="C108" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E108" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+      <c r="C107" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E107" s="65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D108" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
-      <c r="C109" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D109" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E109" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
-      <c r="A110" s="22"/>
-      <c r="B110" s="22"/>
-      <c r="C110" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E110" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+      <c r="C109" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
-      <c r="C111" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D111" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E111" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
-      <c r="A112" s="22"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D112" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E112" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+      <c r="C111" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D111" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
-      <c r="C113" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D113" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E113" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
-      <c r="A114" s="22"/>
-      <c r="B114" s="22"/>
-      <c r="C114" s="29"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="17"/>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
+      <c r="C113" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="16"/>
+    </row>
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
-      <c r="C115" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
-      <c r="A116" s="22"/>
-      <c r="B116" s="22"/>
-      <c r="C116" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D116" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="E116" s="17" t="s">
-        <v>35</v>
+      <c r="C115" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1">
@@ -2320,560 +2536,560 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="63"/>
+      <c r="E117" s="62"/>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="2"/>
-      <c r="E118" s="63"/>
+      <c r="E118" s="62"/>
     </row>
     <row r="119" spans="1:5" s="4" customFormat="1">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="2"/>
-      <c r="E119" s="63"/>
+      <c r="E119" s="62"/>
     </row>
     <row r="120" spans="1:5" s="4" customFormat="1">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="63"/>
+      <c r="E120" s="62"/>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="63"/>
+      <c r="E121" s="62"/>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="63"/>
+      <c r="E122" s="62"/>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="2"/>
-      <c r="E123" s="63"/>
+      <c r="E123" s="62"/>
     </row>
     <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="2"/>
-      <c r="E124" s="63"/>
+      <c r="E124" s="62"/>
     </row>
     <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="2"/>
-      <c r="E125" s="63"/>
+      <c r="E125" s="62"/>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="2"/>
-      <c r="E126" s="63"/>
+      <c r="E126" s="62"/>
     </row>
     <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="63"/>
+      <c r="E127" s="62"/>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="63"/>
+      <c r="E128" s="62"/>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="63"/>
+      <c r="E129" s="62"/>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="2"/>
-      <c r="E130" s="63"/>
+      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="63"/>
+      <c r="E131" s="62"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="63"/>
+      <c r="E132" s="62"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="63"/>
+      <c r="E133" s="62"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="63"/>
+      <c r="E134" s="62"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="63"/>
+      <c r="E135" s="62"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="63"/>
+      <c r="E136" s="62"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="63"/>
+      <c r="E137" s="62"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="63"/>
+      <c r="E138" s="62"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="63"/>
+      <c r="E139" s="62"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="63"/>
+      <c r="E140" s="62"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="63"/>
+      <c r="E141" s="62"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="63"/>
+      <c r="E142" s="62"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="63"/>
+      <c r="E143" s="62"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="63"/>
+      <c r="E144" s="62"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="63"/>
+      <c r="E145" s="62"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="63"/>
+      <c r="E146" s="62"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="63"/>
+      <c r="E147" s="62"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="63"/>
+      <c r="E148" s="62"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="63"/>
+      <c r="E149" s="62"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="63"/>
+      <c r="E150" s="62"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="63"/>
+      <c r="E151" s="62"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="63"/>
+      <c r="E152" s="62"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="63"/>
+      <c r="E153" s="62"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="63"/>
+      <c r="E154" s="62"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="63"/>
+      <c r="E155" s="62"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="63"/>
+      <c r="E156" s="62"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="63"/>
+      <c r="E157" s="62"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="63"/>
+      <c r="E158" s="62"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="63"/>
+      <c r="E159" s="62"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="63"/>
+      <c r="E160" s="62"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="63"/>
+      <c r="E161" s="62"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="63"/>
+      <c r="E162" s="62"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="63"/>
+      <c r="E163" s="62"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="63"/>
+      <c r="E164" s="62"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="63"/>
+      <c r="E165" s="62"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="63"/>
+      <c r="E166" s="62"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="63"/>
+      <c r="E167" s="62"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="63"/>
+      <c r="E168" s="62"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="63"/>
+      <c r="E169" s="62"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="63"/>
+      <c r="E170" s="62"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="63"/>
+      <c r="E171" s="62"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="63"/>
+      <c r="E172" s="62"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="63"/>
+      <c r="E173" s="62"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="63"/>
+      <c r="E174" s="62"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="63"/>
+      <c r="E175" s="62"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="63"/>
+      <c r="E176" s="62"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="63"/>
+      <c r="E177" s="62"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="63"/>
+      <c r="E178" s="62"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="63"/>
+      <c r="E179" s="62"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="63"/>
+      <c r="E180" s="62"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="63"/>
+      <c r="E181" s="62"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="63"/>
+      <c r="E182" s="62"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="63"/>
+      <c r="E183" s="62"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="63"/>
+      <c r="E184" s="62"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="63"/>
+      <c r="E185" s="62"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="63"/>
+      <c r="E186" s="62"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="63"/>
+      <c r="E187" s="62"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="63"/>
+      <c r="E188" s="62"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="63"/>
+      <c r="E189" s="62"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="63"/>
+      <c r="E190" s="62"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="63"/>
+      <c r="E191" s="62"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="63"/>
+      <c r="E192" s="62"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="63"/>
+      <c r="E193" s="62"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="63"/>
+      <c r="E194" s="62"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="63"/>
+      <c r="E195" s="62"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="63"/>
+      <c r="E196" s="62"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
@@ -3192,6 +3408,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3199,11 +3420,6 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Changed ball handler code
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -48,27 +48,15 @@
     <t>Left Front Motor (controller_type)</t>
   </si>
   <si>
-    <t>leftFrontMotor</t>
-  </si>
-  <si>
     <t>Right Front Motor (controller_type)</t>
   </si>
   <si>
-    <t>rightFrontMotor</t>
-  </si>
-  <si>
     <t>Left Rear Motor (controller_type)</t>
   </si>
   <si>
-    <t>leftRearMotor</t>
-  </si>
-  <si>
     <t>Right Rear Motor (controller_type)</t>
   </si>
   <si>
-    <t>rightRearMotor</t>
-  </si>
-  <si>
     <t>Left Drive Encoder</t>
   </si>
   <si>
@@ -264,9 +252,6 @@
     <t>Transmission</t>
   </si>
   <si>
-    <t>transmission</t>
-  </si>
-  <si>
     <t>Kilroy-Laptops</t>
   </si>
   <si>
@@ -357,12 +342,6 @@
     <t>Left Drivers Gear Up</t>
   </si>
   <si>
-    <t>rightDriverCameraSwitchButtonPressed</t>
-  </si>
-  <si>
-    <t>rightOperatorCameraSwitchButtonPressed</t>
-  </si>
-  <si>
     <t>CAN 12</t>
   </si>
   <si>
@@ -430,6 +409,153 @@
   </si>
   <si>
     <t>Left Operator Trigger</t>
+  </si>
+  <si>
+    <t>leftTopMotor</t>
+  </si>
+  <si>
+    <t>rightTopMotor</t>
+  </si>
+  <si>
+    <t>leftBottomMotor</t>
+  </si>
+  <si>
+    <t>rightBottomMotor</t>
+  </si>
+  <si>
+    <t>ballCountInitSwitch</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>spinSwitch</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>floorLight</t>
+  </si>
+  <si>
+    <t>Spin Switch</t>
+  </si>
+  <si>
+    <t>Ball Counter Switch</t>
+  </si>
+  <si>
+    <t>intakePiston</t>
+  </si>
+  <si>
+    <t>Intake Piston</t>
+  </si>
+  <si>
+    <t>rightOperatorCameraSwitchButton</t>
+  </si>
+  <si>
+    <t>rightDriverCameraSwitchButton</t>
+  </si>
+  <si>
+    <t>launchButton</t>
+  </si>
+  <si>
+    <t>launchDisableButton</t>
+  </si>
+  <si>
+    <t>subtractBallButton</t>
+  </si>
+  <si>
+    <t>addBallButton</t>
+  </si>
+  <si>
+    <t>Right 5</t>
+  </si>
+  <si>
+    <t>Right1</t>
+  </si>
+  <si>
+    <t>Right 9</t>
+  </si>
+  <si>
+    <t>Right 8</t>
+  </si>
+  <si>
+    <t>Launch Ball</t>
+  </si>
+  <si>
+    <t>Disable Launch</t>
+  </si>
+  <si>
+    <t>Subtract from Ball Count</t>
+  </si>
+  <si>
+    <t>Add to Ball Count</t>
+  </si>
+  <si>
+    <t>Floor Light</t>
+  </si>
+  <si>
+    <t>launchMotorForward</t>
+  </si>
+  <si>
+    <t>launchMotorBackward</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Intake Motor</t>
+  </si>
+  <si>
+    <t>intakeMotor</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Launch Motor Forward</t>
+  </si>
+  <si>
+    <t>Launch Motor Backward</t>
+  </si>
+  <si>
+    <t>colorWheelMotor</t>
+  </si>
+  <si>
+    <t>Color Wheel Motor</t>
+  </si>
+  <si>
+    <t>5, 4</t>
+  </si>
+  <si>
+    <t>launcher</t>
+  </si>
+  <si>
+    <t>Launcher</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor</t>
+  </si>
+  <si>
+    <t>ultraSonic</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>compressor</t>
+  </si>
+  <si>
+    <t>tankTransmission</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>PCB</t>
   </si>
 </sst>
 </file>
@@ -636,36 +762,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -807,14 +930,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1122,7 +1248,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1132,34 +1258,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="69" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1179,10 +1305,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1193,1126 +1319,1216 @@
       <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19" t="s">
+      <c r="D7" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D10" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="23" customFormat="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="15" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D11" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="64" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="65" t="s">
+      <c r="C12" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+      <c r="E12" s="65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="64"/>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="C14" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="34"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="71" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="70"/>
+      <c r="E19" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="68"/>
+      <c r="E28" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="64" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="66" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" s="64" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="66" t="s">
-        <v>128</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-    </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-    </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-    </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+      <c r="E29" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+      <c r="C30" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="C32" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="21"/>
-    </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="21"/>
-    </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="16"/>
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="21"/>
-    </row>
-    <row r="41" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="17"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="17"/>
-    </row>
-    <row r="44" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="21"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="20"/>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="70" t="s">
+      <c r="A45" s="37"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="68"/>
+      <c r="E45" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A46" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+    </row>
+    <row r="47" spans="1:5" s="4" customFormat="1">
+      <c r="A47" s="49"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="68"/>
+      <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="9" t="s">
+    </row>
+    <row r="51" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A51" s="51"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="52" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
-      <c r="A46" s="47" t="s">
+      <c r="D51" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-    </row>
-    <row r="47" spans="1:5" s="4" customFormat="1">
-      <c r="A47" s="50"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="31"/>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
-      <c r="A48" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="70" t="s">
+      <c r="E51" s="48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="16"/>
+    </row>
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="9" t="s">
+      <c r="D57" s="68"/>
+      <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="53" t="s">
+    <row r="58" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A58" s="51"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="D58" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E58" s="48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="16"/>
+    </row>
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="68"/>
+      <c r="E62" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A63" s="51"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="16"/>
+    </row>
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="16"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
+    </row>
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A68" s="37"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="68"/>
+      <c r="E68" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="16"/>
+    </row>
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="16"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+    </row>
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A73" s="37"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="68"/>
+      <c r="E73" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G73" s="55"/>
+    </row>
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" s="55"/>
+    </row>
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G75" s="55"/>
+    </row>
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A76" s="17"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" s="55"/>
+    </row>
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G77" s="55"/>
+    </row>
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A78" s="37"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="68" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="13"/>
-    </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="70"/>
-      <c r="E57" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A58" s="52"/>
-      <c r="B58" s="52"/>
-      <c r="C58" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="E58" s="49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="13"/>
-    </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A62" s="38"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="D62" s="70"/>
-      <c r="E62" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:8" s="54" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="17"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="55"/>
-    </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A68" s="38"/>
-      <c r="B68" s="38"/>
-      <c r="C68" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="E69" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="42"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="13"/>
-    </row>
-    <row r="72" spans="1:8" s="54" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="17"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55"/>
-    </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A73" s="38"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="D73" s="70"/>
-      <c r="E73" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G73" s="56"/>
-    </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G74" s="56"/>
-    </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E75" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G75" s="56"/>
-    </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D76" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G76" s="56"/>
-    </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
-      <c r="C77" s="29" t="s">
+      <c r="D78" s="68"/>
+      <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E77" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G77" s="56"/>
-    </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A78" s="38"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="70" t="s">
-        <v>57</v>
-      </c>
-      <c r="D78" s="70"/>
-      <c r="E78" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G78" s="56"/>
+      <c r="G78" s="55"/>
     </row>
     <row r="79" spans="1:8" s="4" customFormat="1" ht="25.5">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="D79" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E79" s="33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="54" customFormat="1" ht="25.5">
-      <c r="A80" s="22"/>
-      <c r="B80" s="22"/>
-      <c r="C80" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="D80" s="67" t="s">
-        <v>111</v>
-      </c>
-      <c r="E80" s="64" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
-      <c r="A81" s="58"/>
-      <c r="B81" s="58"/>
-      <c r="C81" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
-      <c r="A82" s="22"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="64" t="s">
+      <c r="A79" s="17"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D80" s="66" t="s">
+        <v>143</v>
+      </c>
+      <c r="E80" s="63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A81" s="57"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D82" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="64" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D83" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="E83" s="66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
-      <c r="A84" s="22"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="17"/>
+      <c r="D81" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E81" s="32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+      <c r="A83" s="42"/>
+      <c r="B83" s="42"/>
+      <c r="C83" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E83" s="65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D84" s="66" t="s">
+        <v>144</v>
+      </c>
+      <c r="E84" s="63" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="85" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A85" s="5"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="32"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="56"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
-      <c r="A86" s="22"/>
-      <c r="B86" s="22"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="17"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E85" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="F85" s="55"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="D86" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="E86" s="63" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
-      <c r="B87" s="18"/>
-      <c r="C87" s="31"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="56"/>
-    </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="17"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="D87" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E87" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="F87" s="55"/>
+    </row>
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="16"/>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="31"/>
-      <c r="D89" s="32"/>
-      <c r="E89" s="57"/>
-      <c r="F89" s="56"/>
-    </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
-      <c r="A90" s="22"/>
-      <c r="B90" s="22"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="55"/>
+    </row>
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="16"/>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="31"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="56"/>
-    </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
-      <c r="A92" s="22"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="17"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="55"/>
+    </row>
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="16"/>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="56"/>
-    </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
-      <c r="A94" s="22"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="17"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="55"/>
+    </row>
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="16"/>
     </row>
     <row r="95" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A95" s="5"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="31"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="56"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="31"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="55"/>
     </row>
     <row r="96" spans="1:6" s="4" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A96" s="22"/>
-      <c r="B96" s="22"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="17"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="16"/>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A97" s="5"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="56"/>
-    </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
-      <c r="A98" s="22"/>
-      <c r="B98" s="22"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="17"/>
-    </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
-      <c r="A99" s="38"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="70" t="s">
+      <c r="B97" s="17"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="55"/>
+    </row>
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="16"/>
+    </row>
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D99" s="68"/>
+      <c r="E99" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G99" s="55"/>
+    </row>
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A100" s="17"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E100" s="41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="16"/>
+    </row>
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A102" s="37"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D102" s="59"/>
+      <c r="E102" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D99" s="70"/>
-      <c r="E99" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G99" s="56"/>
-    </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
-      <c r="A100" s="18"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D100" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="E100" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
-      <c r="A101" s="22"/>
-      <c r="B101" s="22"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="17"/>
-    </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
-      <c r="A102" s="38"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D102" s="60"/>
-      <c r="E102" s="39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    </row>
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
-      <c r="C103" s="42"/>
-      <c r="D103" s="34"/>
-      <c r="E103" s="21"/>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
-      <c r="A104" s="22"/>
-      <c r="B104" s="22"/>
-      <c r="C104" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E104" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+      <c r="C103" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D103" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="E103" s="65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
-      <c r="C105" s="42" t="s">
+      <c r="C105" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D105" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E105" s="60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D105" s="34" t="s">
+      <c r="E106" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="E105" s="61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D106" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E106" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    </row>
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
-      <c r="C107" s="31"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="21"/>
-    </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
-      <c r="A108" s="22"/>
-      <c r="B108" s="22"/>
-      <c r="C108" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D108" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E108" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+      <c r="C107" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E107" s="65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D108" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
-      <c r="C109" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D109" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E109" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
-      <c r="A110" s="22"/>
-      <c r="B110" s="22"/>
-      <c r="C110" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E110" s="17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+      <c r="C109" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
-      <c r="C111" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D111" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E111" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
-      <c r="A112" s="22"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D112" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E112" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+      <c r="C111" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D111" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="E111" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
-      <c r="C113" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D113" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E113" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
-      <c r="A114" s="22"/>
-      <c r="B114" s="22"/>
-      <c r="C114" s="29"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="17"/>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
+      <c r="C113" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="29"/>
+      <c r="E114" s="16"/>
+    </row>
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
-      <c r="C115" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D115" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
-      <c r="A116" s="22"/>
-      <c r="B116" s="22"/>
-      <c r="C116" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D116" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="E116" s="17" t="s">
-        <v>35</v>
+      <c r="C115" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1">
@@ -2320,560 +2536,560 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="63"/>
+      <c r="E117" s="62"/>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="2"/>
-      <c r="E118" s="63"/>
+      <c r="E118" s="62"/>
     </row>
     <row r="119" spans="1:5" s="4" customFormat="1">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="2"/>
-      <c r="E119" s="63"/>
+      <c r="E119" s="62"/>
     </row>
     <row r="120" spans="1:5" s="4" customFormat="1">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="63"/>
+      <c r="E120" s="62"/>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="63"/>
+      <c r="E121" s="62"/>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="63"/>
+      <c r="E122" s="62"/>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="2"/>
-      <c r="E123" s="63"/>
+      <c r="E123" s="62"/>
     </row>
     <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="2"/>
-      <c r="E124" s="63"/>
+      <c r="E124" s="62"/>
     </row>
     <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="2"/>
-      <c r="E125" s="63"/>
+      <c r="E125" s="62"/>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="2"/>
-      <c r="E126" s="63"/>
+      <c r="E126" s="62"/>
     </row>
     <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="63"/>
+      <c r="E127" s="62"/>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="63"/>
+      <c r="E128" s="62"/>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="63"/>
+      <c r="E129" s="62"/>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="2"/>
-      <c r="E130" s="63"/>
+      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="63"/>
+      <c r="E131" s="62"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="63"/>
+      <c r="E132" s="62"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="63"/>
+      <c r="E133" s="62"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="63"/>
+      <c r="E134" s="62"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="63"/>
+      <c r="E135" s="62"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="63"/>
+      <c r="E136" s="62"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="63"/>
+      <c r="E137" s="62"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="63"/>
+      <c r="E138" s="62"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="63"/>
+      <c r="E139" s="62"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="63"/>
+      <c r="E140" s="62"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="63"/>
+      <c r="E141" s="62"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="63"/>
+      <c r="E142" s="62"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="63"/>
+      <c r="E143" s="62"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="63"/>
+      <c r="E144" s="62"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="63"/>
+      <c r="E145" s="62"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="63"/>
+      <c r="E146" s="62"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="63"/>
+      <c r="E147" s="62"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="63"/>
+      <c r="E148" s="62"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="63"/>
+      <c r="E149" s="62"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="63"/>
+      <c r="E150" s="62"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="63"/>
+      <c r="E151" s="62"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="63"/>
+      <c r="E152" s="62"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="63"/>
+      <c r="E153" s="62"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="63"/>
+      <c r="E154" s="62"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="63"/>
+      <c r="E155" s="62"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="63"/>
+      <c r="E156" s="62"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="63"/>
+      <c r="E157" s="62"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="63"/>
+      <c r="E158" s="62"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="63"/>
+      <c r="E159" s="62"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="63"/>
+      <c r="E160" s="62"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="63"/>
+      <c r="E161" s="62"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="63"/>
+      <c r="E162" s="62"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="63"/>
+      <c r="E163" s="62"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="63"/>
+      <c r="E164" s="62"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="63"/>
+      <c r="E165" s="62"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="63"/>
+      <c r="E166" s="62"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="63"/>
+      <c r="E167" s="62"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="63"/>
+      <c r="E168" s="62"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="63"/>
+      <c r="E169" s="62"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="63"/>
+      <c r="E170" s="62"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="63"/>
+      <c r="E171" s="62"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="63"/>
+      <c r="E172" s="62"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="63"/>
+      <c r="E173" s="62"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="63"/>
+      <c r="E174" s="62"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="63"/>
+      <c r="E175" s="62"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="63"/>
+      <c r="E176" s="62"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="63"/>
+      <c r="E177" s="62"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="63"/>
+      <c r="E178" s="62"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="63"/>
+      <c r="E179" s="62"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="63"/>
+      <c r="E180" s="62"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="63"/>
+      <c r="E181" s="62"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="63"/>
+      <c r="E182" s="62"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="63"/>
+      <c r="E183" s="62"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="63"/>
+      <c r="E184" s="62"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="63"/>
+      <c r="E185" s="62"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="63"/>
+      <c r="E186" s="62"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="63"/>
+      <c r="E187" s="62"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="63"/>
+      <c r="E188" s="62"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="63"/>
+      <c r="E189" s="62"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="63"/>
+      <c r="E190" s="62"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="63"/>
+      <c r="E191" s="62"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="63"/>
+      <c r="E192" s="62"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="63"/>
+      <c r="E193" s="62"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="63"/>
+      <c r="E194" s="62"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="63"/>
+      <c r="E195" s="62"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="63"/>
+      <c r="E196" s="62"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
@@ -3192,6 +3408,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3199,11 +3420,6 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added double throw switch
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>Double Throw Switch</t>
+  </si>
+  <si>
+    <t>unknown at this time</t>
+  </si>
+  <si>
+    <t>11/12</t>
   </si>
 </sst>
 </file>
@@ -930,17 +939,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,7 +1257,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1258,22 +1267,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1285,7 +1294,7 @@
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1305,10 +1314,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
@@ -1365,7 +1374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -1381,7 +1390,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="64" t="s">
@@ -1397,7 +1406,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1413,7 +1422,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="64" t="s">
@@ -1426,7 +1435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1439,7 +1448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="64" t="s">
@@ -1452,7 +1461,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1465,7 +1474,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="64" t="s">
@@ -1478,7 +1487,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="64" t="s">
@@ -1491,7 +1500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="64" t="s">
@@ -1504,7 +1513,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1514,15 +1523,15 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="64" t="s">
@@ -1535,7 +1544,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
@@ -1548,7 +1557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="64" t="s">
@@ -1564,7 +1573,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
@@ -1580,7 +1589,7 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
       <c r="C24" s="64" t="s">
@@ -1596,7 +1605,7 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1606,7 +1615,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1616,7 +1625,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1626,18 +1635,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1650,7 +1659,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1663,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="64" t="s">
@@ -1676,7 +1685,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="32" spans="1:8" s="4" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
@@ -1689,56 +1698,62 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="C33" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1776,15 +1791,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1817,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1813,7 +1828,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1823,10 +1838,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
@@ -1857,28 +1872,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1888,10 +1903,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1909,42 +1924,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="71" t="s">
+      <c r="C63" s="68" t="s">
         <v>141</v>
       </c>
       <c r="D63" s="47" t="s">
@@ -1954,21 +1969,21 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1984,18 +1999,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2008,14 +2023,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2031,19 +2046,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2057,7 +2072,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2071,7 +2086,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2085,7 +2100,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2099,13 +2114,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
@@ -2150,7 +2165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="63" t="s">
@@ -2163,7 +2178,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
@@ -2176,7 +2191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="64" t="s">
@@ -2203,7 +2218,7 @@
       </c>
       <c r="F85" s="55"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="64" t="s">
@@ -2230,7 +2245,7 @@
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="28"/>
@@ -2245,7 +2260,7 @@
       <c r="E89" s="56"/>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="28"/>
@@ -2260,7 +2275,7 @@
       <c r="E91" s="20"/>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="28"/>
@@ -2275,7 +2290,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2305,26 +2320,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="70"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2337,14 +2352,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2355,7 +2370,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
@@ -2368,7 +2383,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2381,7 +2396,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2394,7 +2409,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2407,7 +2422,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
@@ -2420,7 +2435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2433,7 +2448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2446,7 +2461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2459,7 +2474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
@@ -2472,7 +2487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2485,7 +2500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2498,14 +2513,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="28"/>
       <c r="D114" s="29"/>
       <c r="E114" s="16"/>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="30" t="s">
@@ -2518,7 +2533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="28" t="s">
@@ -3408,11 +3423,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3420,6 +3430,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added outtake code to ballhandler and teleop
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>Double Throw Switch</t>
+  </si>
+  <si>
+    <t>unknown at this time</t>
+  </si>
+  <si>
+    <t>11/12</t>
   </si>
 </sst>
 </file>
@@ -930,17 +939,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,7 +1257,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1258,22 +1267,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1285,7 +1294,7 @@
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1305,10 +1314,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
@@ -1365,7 +1374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -1381,7 +1390,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="64" t="s">
@@ -1397,7 +1406,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1413,7 +1422,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="64" t="s">
@@ -1426,7 +1435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1439,7 +1448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="64" t="s">
@@ -1452,7 +1461,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1465,7 +1474,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="64" t="s">
@@ -1478,7 +1487,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="64" t="s">
@@ -1491,7 +1500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="64" t="s">
@@ -1504,7 +1513,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1514,15 +1523,15 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="64" t="s">
@@ -1535,7 +1544,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
@@ -1548,7 +1557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="64" t="s">
@@ -1564,7 +1573,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
@@ -1580,7 +1589,7 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
       <c r="C24" s="64" t="s">
@@ -1596,7 +1605,7 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1606,7 +1615,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1616,7 +1625,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1626,18 +1635,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1650,7 +1659,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1663,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="64" t="s">
@@ -1676,7 +1685,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="32" spans="1:8" s="4" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
@@ -1689,56 +1698,62 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="C33" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1776,15 +1791,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1817,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1813,7 +1828,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1823,10 +1838,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
@@ -1857,28 +1872,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1888,10 +1903,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1909,42 +1924,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="71" t="s">
+      <c r="C63" s="68" t="s">
         <v>141</v>
       </c>
       <c r="D63" s="47" t="s">
@@ -1954,21 +1969,21 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1984,18 +1999,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2008,14 +2023,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2031,19 +2046,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2057,7 +2072,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2071,7 +2086,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2085,7 +2100,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2099,13 +2114,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
@@ -2150,7 +2165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="63" t="s">
@@ -2163,7 +2178,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
@@ -2176,7 +2191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="64" t="s">
@@ -2203,7 +2218,7 @@
       </c>
       <c r="F85" s="55"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="64" t="s">
@@ -2230,7 +2245,7 @@
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="28"/>
@@ -2245,7 +2260,7 @@
       <c r="E89" s="56"/>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="28"/>
@@ -2260,7 +2275,7 @@
       <c r="E91" s="20"/>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="28"/>
@@ -2275,7 +2290,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2305,26 +2320,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="70"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2337,14 +2352,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2355,7 +2370,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
@@ -2368,7 +2383,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2381,7 +2396,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2394,7 +2409,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2407,7 +2422,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
@@ -2420,7 +2435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2433,7 +2448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2446,7 +2461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2459,7 +2474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
@@ -2472,7 +2487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2485,7 +2500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2498,14 +2513,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="28"/>
       <c r="D114" s="29"/>
       <c r="E114" s="16"/>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="30" t="s">
@@ -2518,7 +2533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="28" t="s">
@@ -3408,11 +3423,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3420,6 +3430,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added correct equitment list
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -556,6 +556,15 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>Double Throw Switch</t>
+  </si>
+  <si>
+    <t>unknown at this time</t>
+  </si>
+  <si>
+    <t>11/12</t>
   </si>
 </sst>
 </file>
@@ -930,17 +939,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,7 +1257,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1258,22 +1267,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1285,7 +1294,7 @@
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1305,10 +1314,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1352,7 +1361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
@@ -1365,7 +1374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
@@ -1381,7 +1390,7 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="64" t="s">
@@ -1397,7 +1406,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1413,7 +1422,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="64" t="s">
@@ -1426,7 +1435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1439,7 +1448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="64" t="s">
@@ -1452,7 +1461,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1465,7 +1474,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="64" t="s">
@@ -1478,7 +1487,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="64" t="s">
@@ -1491,7 +1500,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="64" t="s">
@@ -1504,7 +1513,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1514,15 +1523,15 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="64" t="s">
@@ -1535,7 +1544,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
@@ -1548,7 +1557,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="64" t="s">
@@ -1564,7 +1573,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
@@ -1580,7 +1589,7 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
       <c r="C24" s="64" t="s">
@@ -1596,7 +1605,7 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1606,7 +1615,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1616,7 +1625,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1626,18 +1635,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1650,7 +1659,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1663,7 +1672,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="64" t="s">
@@ -1676,7 +1685,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="32" spans="1:8" s="4" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
@@ -1689,56 +1698,62 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="C33" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1776,15 +1791,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1817,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1813,7 +1828,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1823,10 +1838,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
@@ -1857,28 +1872,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1888,10 +1903,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1909,42 +1924,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="71" t="s">
+      <c r="C63" s="68" t="s">
         <v>141</v>
       </c>
       <c r="D63" s="47" t="s">
@@ -1954,21 +1969,21 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1984,18 +1999,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2008,14 +2023,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2031,19 +2046,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2057,7 +2072,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2071,7 +2086,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2085,7 +2100,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2099,13 +2114,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
@@ -2150,7 +2165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="63" t="s">
@@ -2163,7 +2178,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
@@ -2176,7 +2191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="84" spans="1:6" s="4" customFormat="1">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="64" t="s">
@@ -2203,7 +2218,7 @@
       </c>
       <c r="F85" s="55"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="64" t="s">
@@ -2230,7 +2245,7 @@
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="28"/>
@@ -2245,7 +2260,7 @@
       <c r="E89" s="56"/>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="28"/>
@@ -2260,7 +2275,7 @@
       <c r="E91" s="20"/>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="28"/>
@@ -2275,7 +2290,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2305,26 +2320,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="70"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2337,14 +2352,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2355,7 +2370,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
@@ -2368,7 +2383,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2381,7 +2396,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2394,7 +2409,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2407,7 +2422,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
@@ -2420,7 +2435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2433,7 +2448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2446,7 +2461,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2459,7 +2474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
@@ -2472,7 +2487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2485,7 +2500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2498,14 +2513,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="28"/>
       <c r="D114" s="29"/>
       <c r="E114" s="16"/>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="30" t="s">
@@ -2518,7 +2533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="28" t="s">
@@ -3408,11 +3423,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3420,6 +3430,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Finished outtake and fixed stuff in teleop/harware
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="203">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Change Camera Operator Side</t>
   </si>
   <si>
-    <t>Right 10</t>
-  </si>
-  <si>
-    <t>Right 3</t>
-  </si>
-  <si>
     <t>Change Camera Driver Side</t>
   </si>
   <si>
@@ -468,18 +462,6 @@
     <t>addBallButton</t>
   </si>
   <si>
-    <t>Right 5</t>
-  </si>
-  <si>
-    <t>Right1</t>
-  </si>
-  <si>
-    <t>Right 9</t>
-  </si>
-  <si>
-    <t>Right 8</t>
-  </si>
-  <si>
     <t>Launch Ball</t>
   </si>
   <si>
@@ -565,6 +547,90 @@
   </si>
   <si>
     <t>11/12</t>
+  </si>
+  <si>
+    <t>Drive Delay Timer</t>
+  </si>
+  <si>
+    <t>Launch Delay Timer</t>
+  </si>
+  <si>
+    <t>driveDelayTimer</t>
+  </si>
+  <si>
+    <t>launchDelayTimer</t>
+  </si>
+  <si>
+    <t>climbUpButton</t>
+  </si>
+  <si>
+    <t>Right Operator 3</t>
+  </si>
+  <si>
+    <t>climbDownButton</t>
+  </si>
+  <si>
+    <t>Climb Down Button</t>
+  </si>
+  <si>
+    <t>Climb Up Button</t>
+  </si>
+  <si>
+    <t>Outtake Button</t>
+  </si>
+  <si>
+    <t>outtakeButton</t>
+  </si>
+  <si>
+    <t>Left Operator 2</t>
+  </si>
+  <si>
+    <t>Right Operator 2</t>
+  </si>
+  <si>
+    <t>Ball Counter</t>
+  </si>
+  <si>
+    <t>ballCounter</t>
+  </si>
+  <si>
+    <t>Right Operator 5</t>
+  </si>
+  <si>
+    <t>Right Operator 8</t>
+  </si>
+  <si>
+    <t>Right Operator 9</t>
+  </si>
+  <si>
+    <t>Right Driver 3</t>
+  </si>
+  <si>
+    <t>Right Operator 10</t>
+  </si>
+  <si>
+    <t>Climb Timer</t>
+  </si>
+  <si>
+    <t>climbTimer</t>
+  </si>
+  <si>
+    <t>Close Climb Servo</t>
+  </si>
+  <si>
+    <t>closeClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator 4</t>
+  </si>
+  <si>
+    <t>Open Climb Servo</t>
+  </si>
+  <si>
+    <t>openClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator Trigger</t>
   </si>
 </sst>
 </file>
@@ -574,7 +640,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,6 +701,14 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF993300"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -736,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -909,9 +983,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,14 +1013,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,7 +1343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,36 +1351,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK241"/>
+  <dimension ref="A1:AMK255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1314,10 +1400,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1329,10 +1415,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>109</v>
+        <v>127</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1342,10 +1428,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>108</v>
+        <v>128</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1355,58 +1441,58 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="22" customFormat="1">
+        <v>129</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
+        <v>130</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="63" t="s">
+      <c r="C9" s="63" t="s">
         <v>159</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>153</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1415,105 +1501,105 @@
       <c r="D10" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="64" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+        <v>96</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+      <c r="C13" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="64" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
+      <c r="C15" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="63" t="s">
+      <c r="C16" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+      <c r="E16" s="62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="C17" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1523,99 +1609,99 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+      <c r="C20" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+        <v>116</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="63" t="s">
-        <v>122</v>
+      <c r="C22" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>120</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>119</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>176</v>
+      <c r="C24" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>170</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="65"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1625,7 +1711,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1635,18 +1721,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="70"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1659,7 +1745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1672,88 +1758,88 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
-      <c r="C31" s="64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+      <c r="C31" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
+        <v>133</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>179</v>
-      </c>
-      <c r="E33" s="63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="C33" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1791,15 +1877,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="70"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1817,7 +1903,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1914,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1838,10 +1924,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="70"/>
+      <c r="D50" s="68"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1859,41 +1945,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1903,10 +1989,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="70" t="s">
+      <c r="C57" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="70"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1924,66 +2010,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="70" t="s">
+      <c r="C62" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="70"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="68" t="s">
-        <v>141</v>
+      <c r="C63" s="67" t="s">
+        <v>139</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="E63" s="63" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
+        <v>138</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1999,18 +2085,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="70" t="s">
+      <c r="C68" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="70"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2023,14 +2109,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2046,19 +2132,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="70" t="s">
+      <c r="C73" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="70"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2072,7 +2158,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2086,7 +2172,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2100,7 +2186,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2114,13 +2200,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="70" t="s">
+      <c r="C78" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="70"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2133,154 +2219,184 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
-      <c r="C80" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="D80" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" s="63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
+      <c r="C80" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D80" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" s="62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
-      <c r="C82" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D82" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="E82" s="63" t="s">
+      <c r="C82" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="65" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
+      <c r="E82" s="62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D83" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="E83" s="65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
+    </row>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
-      <c r="C84" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="D84" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="E84" s="63" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A85" s="5"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="E85" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="F85" s="55"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
+      <c r="C84" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="62" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="75" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A85" s="57"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F85" s="74"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
-      <c r="C86" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="D86" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="E86" s="63" t="s">
-        <v>151</v>
+      <c r="C86" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" s="62" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E87" s="65" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="E87" s="64" t="s">
+        <v>192</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="16"/>
+      <c r="C88" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88" s="62" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="31"/>
-      <c r="E89" s="56"/>
+      <c r="C89" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="E89" s="56" t="s">
+        <v>187</v>
+      </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="16"/>
+      <c r="C90" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="D90" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E90" s="62" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="20"/>
+      <c r="C91" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" s="64" t="s">
+        <v>199</v>
+      </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="16"/>
+      <c r="C92" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="D92" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E92" s="62" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
@@ -2290,7 +2406,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2320,26 +2436,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="70" t="s">
+      <c r="C99" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="70"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2352,38 +2468,38 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="58"/>
       <c r="E102" s="38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D103" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="E103" s="65" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
+        <v>168</v>
+      </c>
+      <c r="E103" s="64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2396,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2405,11 +2521,11 @@
       <c r="D105" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E105" s="60" t="s">
+      <c r="E105" s="59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2418,24 +2534,24 @@
       <c r="D106" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E106" s="61" t="s">
+      <c r="E106" s="60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E107" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2448,7 +2564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2461,7 +2577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2474,20 +2590,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2500,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2513,696 +2629,720 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="29"/>
-      <c r="E114" s="16"/>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E115" s="30" t="s">
+      <c r="C114" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D114" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A115" s="17"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
-      <c r="C116" s="28" t="s">
+      <c r="C116" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="D116" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="E116" s="62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D117" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E117" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="16"/>
+    </row>
+    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A119" s="17"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="41"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="20"/>
+    </row>
+    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="16"/>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="41"/>
+      <c r="D121" s="42"/>
+      <c r="E121" s="20"/>
+    </row>
+    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="16"/>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A123" s="17"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="42"/>
+      <c r="E123" s="20"/>
+    </row>
+    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="16"/>
+    </row>
+    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="20"/>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="16"/>
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A127" s="17"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="42"/>
+      <c r="E127" s="20"/>
+    </row>
+    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="16"/>
+    </row>
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D116" s="29" t="s">
+      <c r="D130" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="E130" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="62"/>
-    </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="62"/>
-    </row>
-    <row r="119" spans="1:5" s="4" customFormat="1">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="62"/>
-    </row>
-    <row r="120" spans="1:5" s="4" customFormat="1">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="62"/>
-    </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="62"/>
-    </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="62"/>
-    </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="62"/>
-    </row>
-    <row r="124" spans="1:5" s="4" customFormat="1">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="62"/>
-    </row>
-    <row r="125" spans="1:5" s="4" customFormat="1">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="62"/>
-    </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="62"/>
-    </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="62"/>
-    </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="62"/>
-    </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="62"/>
-    </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="62"/>
+      <c r="E131" s="61"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="62"/>
+      <c r="E132" s="61"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="62"/>
+      <c r="E133" s="61"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="62"/>
+      <c r="E134" s="61"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="62"/>
+      <c r="E135" s="61"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="62"/>
+      <c r="E136" s="61"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="62"/>
+      <c r="E137" s="61"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="62"/>
+      <c r="E138" s="61"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="62"/>
+      <c r="E139" s="61"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="62"/>
+      <c r="E140" s="61"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="62"/>
+      <c r="E141" s="61"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="62"/>
+      <c r="E142" s="61"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="62"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="62"/>
+      <c r="E144" s="61"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="62"/>
+      <c r="E145" s="61"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="62"/>
+      <c r="E146" s="61"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="62"/>
+      <c r="E147" s="61"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="62"/>
+      <c r="E148" s="61"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="62"/>
+      <c r="E149" s="61"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="62"/>
+      <c r="E150" s="61"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="62"/>
+      <c r="E151" s="61"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="62"/>
+      <c r="E152" s="61"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="62"/>
+      <c r="E153" s="61"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="62"/>
+      <c r="E154" s="61"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="62"/>
+      <c r="E155" s="61"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="62"/>
+      <c r="E156" s="61"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="62"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="62"/>
+      <c r="E158" s="61"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="62"/>
+      <c r="E159" s="61"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="62"/>
+      <c r="E160" s="61"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="62"/>
+      <c r="E161" s="61"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="62"/>
+      <c r="E162" s="61"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="62"/>
+      <c r="E163" s="61"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="62"/>
+      <c r="E164" s="61"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="62"/>
+      <c r="E165" s="61"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="62"/>
+      <c r="E166" s="61"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="62"/>
+      <c r="E167" s="61"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="62"/>
+      <c r="E168" s="61"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="62"/>
+      <c r="E169" s="61"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="62"/>
+      <c r="E170" s="61"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="62"/>
+      <c r="E171" s="61"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="62"/>
+      <c r="E172" s="61"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="62"/>
+      <c r="E173" s="61"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="62"/>
+      <c r="E174" s="61"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="62"/>
+      <c r="E175" s="61"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="62"/>
+      <c r="E176" s="61"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="62"/>
+      <c r="E177" s="61"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="62"/>
+      <c r="E178" s="61"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="62"/>
+      <c r="E179" s="61"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="62"/>
+      <c r="E180" s="61"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="62"/>
+      <c r="E181" s="61"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="62"/>
+      <c r="E182" s="61"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="62"/>
+      <c r="E183" s="61"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="62"/>
+      <c r="E184" s="61"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="62"/>
+      <c r="E185" s="61"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="62"/>
+      <c r="E186" s="61"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="62"/>
+      <c r="E187" s="61"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="62"/>
+      <c r="E188" s="61"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="62"/>
+      <c r="E189" s="61"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="62"/>
+      <c r="E190" s="61"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="62"/>
+      <c r="E191" s="61"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="62"/>
+      <c r="E192" s="61"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="62"/>
+      <c r="E193" s="61"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="62"/>
+      <c r="E194" s="61"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="62"/>
+      <c r="E195" s="61"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="62"/>
+      <c r="E196" s="61"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
-      <c r="E197" s="3"/>
+      <c r="E197" s="61"/>
     </row>
     <row r="198" spans="1:5" s="4" customFormat="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
-      <c r="E198" s="3"/>
+      <c r="E198" s="61"/>
     </row>
     <row r="199" spans="1:5" s="4" customFormat="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
-      <c r="E199" s="3"/>
+      <c r="E199" s="61"/>
     </row>
     <row r="200" spans="1:5" s="4" customFormat="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
-      <c r="E200" s="3"/>
+      <c r="E200" s="61"/>
     </row>
     <row r="201" spans="1:5" s="4" customFormat="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
-      <c r="E201" s="3"/>
+      <c r="E201" s="61"/>
     </row>
     <row r="202" spans="1:5" s="4" customFormat="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
-      <c r="E202" s="3"/>
+      <c r="E202" s="61"/>
     </row>
     <row r="203" spans="1:5" s="4" customFormat="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
-      <c r="E203" s="3"/>
+      <c r="E203" s="61"/>
     </row>
     <row r="204" spans="1:5" s="4" customFormat="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
-      <c r="E204" s="3"/>
+      <c r="E204" s="61"/>
     </row>
     <row r="205" spans="1:5" s="4" customFormat="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
-      <c r="E205" s="3"/>
+      <c r="E205" s="61"/>
     </row>
     <row r="206" spans="1:5" s="4" customFormat="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
-      <c r="E206" s="3"/>
+      <c r="E206" s="61"/>
     </row>
     <row r="207" spans="1:5" s="4" customFormat="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
-      <c r="E207" s="3"/>
+      <c r="E207" s="61"/>
     </row>
     <row r="208" spans="1:5" s="4" customFormat="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
-      <c r="E208" s="3"/>
+      <c r="E208" s="61"/>
     </row>
     <row r="209" spans="1:5" s="4" customFormat="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
-      <c r="E209" s="3"/>
+      <c r="E209" s="61"/>
     </row>
     <row r="210" spans="1:5" s="4" customFormat="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
-      <c r="E210" s="3"/>
+      <c r="E210" s="61"/>
     </row>
     <row r="211" spans="1:5" s="4" customFormat="1">
       <c r="A211" s="1"/>
@@ -3421,8 +3561,111 @@
       <c r="D241" s="2"/>
       <c r="E241" s="3"/>
     </row>
+    <row r="242" spans="1:5" s="4" customFormat="1">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="3"/>
+    </row>
+    <row r="243" spans="1:5" s="4" customFormat="1">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="2"/>
+      <c r="E243" s="3"/>
+    </row>
+    <row r="244" spans="1:5" s="4" customFormat="1">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="3"/>
+    </row>
+    <row r="245" spans="1:5" s="4" customFormat="1">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="2"/>
+      <c r="E245" s="3"/>
+    </row>
+    <row r="246" spans="1:5" s="4" customFormat="1">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="2"/>
+      <c r="E246" s="3"/>
+    </row>
+    <row r="247" spans="1:5" s="4" customFormat="1">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="2"/>
+      <c r="E247" s="3"/>
+    </row>
+    <row r="248" spans="1:5" s="4" customFormat="1">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="3"/>
+    </row>
+    <row r="249" spans="1:5" s="4" customFormat="1">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="3"/>
+    </row>
+    <row r="250" spans="1:5" s="4" customFormat="1">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="2"/>
+      <c r="E250" s="3"/>
+    </row>
+    <row r="251" spans="1:5" s="4" customFormat="1">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="2"/>
+      <c r="E251" s="3"/>
+    </row>
+    <row r="252" spans="1:5" s="4" customFormat="1">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="2"/>
+      <c r="E252" s="3"/>
+    </row>
+    <row r="253" spans="1:5" s="4" customFormat="1">
+      <c r="A253" s="1"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="2"/>
+      <c r="E253" s="3"/>
+    </row>
+    <row r="254" spans="1:5" s="4" customFormat="1">
+      <c r="A254" s="1"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="2"/>
+      <c r="E254" s="3"/>
+    </row>
+    <row r="255" spans="1:5" s="4" customFormat="1">
+      <c r="A255" s="1"/>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="2"/>
+      <c r="E255" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3430,13 +3673,8 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed auto to work with the launcher
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="203">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Change Camera Operator Side</t>
   </si>
   <si>
-    <t>Right 10</t>
-  </si>
-  <si>
-    <t>Right 3</t>
-  </si>
-  <si>
     <t>Change Camera Driver Side</t>
   </si>
   <si>
@@ -468,18 +462,6 @@
     <t>addBallButton</t>
   </si>
   <si>
-    <t>Right 5</t>
-  </si>
-  <si>
-    <t>Right1</t>
-  </si>
-  <si>
-    <t>Right 9</t>
-  </si>
-  <si>
-    <t>Right 8</t>
-  </si>
-  <si>
     <t>Launch Ball</t>
   </si>
   <si>
@@ -565,6 +547,90 @@
   </si>
   <si>
     <t>11/12</t>
+  </si>
+  <si>
+    <t>Drive Delay Timer</t>
+  </si>
+  <si>
+    <t>Launch Delay Timer</t>
+  </si>
+  <si>
+    <t>driveDelayTimer</t>
+  </si>
+  <si>
+    <t>launchDelayTimer</t>
+  </si>
+  <si>
+    <t>climbUpButton</t>
+  </si>
+  <si>
+    <t>Right Operator 3</t>
+  </si>
+  <si>
+    <t>climbDownButton</t>
+  </si>
+  <si>
+    <t>Climb Down Button</t>
+  </si>
+  <si>
+    <t>Climb Up Button</t>
+  </si>
+  <si>
+    <t>Outtake Button</t>
+  </si>
+  <si>
+    <t>outtakeButton</t>
+  </si>
+  <si>
+    <t>Left Operator 2</t>
+  </si>
+  <si>
+    <t>Right Operator 2</t>
+  </si>
+  <si>
+    <t>Ball Counter</t>
+  </si>
+  <si>
+    <t>ballCounter</t>
+  </si>
+  <si>
+    <t>Right Operator 5</t>
+  </si>
+  <si>
+    <t>Right Operator 8</t>
+  </si>
+  <si>
+    <t>Right Operator 9</t>
+  </si>
+  <si>
+    <t>Right Driver 3</t>
+  </si>
+  <si>
+    <t>Right Operator 10</t>
+  </si>
+  <si>
+    <t>Climb Timer</t>
+  </si>
+  <si>
+    <t>climbTimer</t>
+  </si>
+  <si>
+    <t>Close Climb Servo</t>
+  </si>
+  <si>
+    <t>closeClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator 4</t>
+  </si>
+  <si>
+    <t>Open Climb Servo</t>
+  </si>
+  <si>
+    <t>openClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator Trigger</t>
   </si>
 </sst>
 </file>
@@ -574,7 +640,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,6 +701,14 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF993300"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -736,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -909,9 +983,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,14 +1013,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,7 +1343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,36 +1351,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK241"/>
+  <dimension ref="A1:AMK255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1314,10 +1400,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1329,10 +1415,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>109</v>
+        <v>127</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1342,10 +1428,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>108</v>
+        <v>128</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1355,58 +1441,58 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="22" customFormat="1">
+        <v>129</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
+        <v>130</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="63" t="s">
+      <c r="C9" s="63" t="s">
         <v>159</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>153</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1415,105 +1501,105 @@
       <c r="D10" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="64" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+        <v>96</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+      <c r="C13" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="64" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
+      <c r="C15" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="63" t="s">
+      <c r="C16" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+      <c r="E16" s="62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="C17" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1523,99 +1609,99 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+      <c r="C20" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+        <v>116</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="63" t="s">
-        <v>122</v>
+      <c r="C22" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>120</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>119</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>176</v>
+      <c r="C24" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>170</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="65"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1625,7 +1711,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1635,18 +1721,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="70"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1659,7 +1745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1672,88 +1758,88 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
-      <c r="C31" s="64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+      <c r="C31" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
+        <v>133</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>179</v>
-      </c>
-      <c r="E33" s="63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="C33" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1791,15 +1877,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="70"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1817,7 +1903,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1914,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1838,10 +1924,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="70"/>
+      <c r="D50" s="68"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1859,41 +1945,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1903,10 +1989,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="70" t="s">
+      <c r="C57" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="70"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1924,66 +2010,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="70" t="s">
+      <c r="C62" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="70"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="68" t="s">
-        <v>141</v>
+      <c r="C63" s="67" t="s">
+        <v>139</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="E63" s="63" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
+        <v>138</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1999,18 +2085,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="70" t="s">
+      <c r="C68" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="70"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2023,14 +2109,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2046,19 +2132,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="70" t="s">
+      <c r="C73" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="70"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2072,7 +2158,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2086,7 +2172,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2100,7 +2186,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2114,13 +2200,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="70" t="s">
+      <c r="C78" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="70"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2133,154 +2219,184 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
-      <c r="C80" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="D80" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" s="63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
+      <c r="C80" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D80" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" s="62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
-      <c r="C82" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D82" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="E82" s="63" t="s">
+      <c r="C82" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="65" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
+      <c r="E82" s="62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D83" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="E83" s="65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
+    </row>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
-      <c r="C84" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="D84" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="E84" s="63" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A85" s="5"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="E85" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="F85" s="55"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
+      <c r="C84" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="62" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="75" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A85" s="57"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F85" s="74"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
-      <c r="C86" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="D86" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="E86" s="63" t="s">
-        <v>151</v>
+      <c r="C86" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" s="62" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E87" s="65" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="E87" s="64" t="s">
+        <v>192</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="16"/>
+      <c r="C88" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88" s="62" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="31"/>
-      <c r="E89" s="56"/>
+      <c r="C89" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="E89" s="56" t="s">
+        <v>187</v>
+      </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="16"/>
+      <c r="C90" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="D90" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E90" s="62" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="20"/>
+      <c r="C91" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" s="64" t="s">
+        <v>199</v>
+      </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="16"/>
+      <c r="C92" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="D92" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E92" s="62" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
@@ -2290,7 +2406,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2320,26 +2436,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="70" t="s">
+      <c r="C99" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="70"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2352,38 +2468,38 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="58"/>
       <c r="E102" s="38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D103" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="E103" s="65" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
+        <v>168</v>
+      </c>
+      <c r="E103" s="64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2396,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2405,11 +2521,11 @@
       <c r="D105" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E105" s="60" t="s">
+      <c r="E105" s="59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2418,24 +2534,24 @@
       <c r="D106" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E106" s="61" t="s">
+      <c r="E106" s="60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E107" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2448,7 +2564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2461,7 +2577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2474,20 +2590,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2500,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2513,696 +2629,720 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="29"/>
-      <c r="E114" s="16"/>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E115" s="30" t="s">
+      <c r="C114" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D114" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A115" s="17"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
-      <c r="C116" s="28" t="s">
+      <c r="C116" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="D116" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="E116" s="62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D117" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E117" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="16"/>
+    </row>
+    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A119" s="17"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="41"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="20"/>
+    </row>
+    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="16"/>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="41"/>
+      <c r="D121" s="42"/>
+      <c r="E121" s="20"/>
+    </row>
+    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="16"/>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A123" s="17"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="42"/>
+      <c r="E123" s="20"/>
+    </row>
+    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="16"/>
+    </row>
+    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="20"/>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="16"/>
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A127" s="17"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="42"/>
+      <c r="E127" s="20"/>
+    </row>
+    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="16"/>
+    </row>
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D116" s="29" t="s">
+      <c r="D130" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="E130" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="62"/>
-    </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="62"/>
-    </row>
-    <row r="119" spans="1:5" s="4" customFormat="1">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="62"/>
-    </row>
-    <row r="120" spans="1:5" s="4" customFormat="1">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="62"/>
-    </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="62"/>
-    </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="62"/>
-    </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="62"/>
-    </row>
-    <row r="124" spans="1:5" s="4" customFormat="1">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="62"/>
-    </row>
-    <row r="125" spans="1:5" s="4" customFormat="1">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="62"/>
-    </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="62"/>
-    </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="62"/>
-    </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="62"/>
-    </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="62"/>
-    </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="62"/>
+      <c r="E131" s="61"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="62"/>
+      <c r="E132" s="61"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="62"/>
+      <c r="E133" s="61"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="62"/>
+      <c r="E134" s="61"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="62"/>
+      <c r="E135" s="61"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="62"/>
+      <c r="E136" s="61"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="62"/>
+      <c r="E137" s="61"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="62"/>
+      <c r="E138" s="61"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="62"/>
+      <c r="E139" s="61"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="62"/>
+      <c r="E140" s="61"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="62"/>
+      <c r="E141" s="61"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="62"/>
+      <c r="E142" s="61"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="62"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="62"/>
+      <c r="E144" s="61"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="62"/>
+      <c r="E145" s="61"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="62"/>
+      <c r="E146" s="61"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="62"/>
+      <c r="E147" s="61"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="62"/>
+      <c r="E148" s="61"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="62"/>
+      <c r="E149" s="61"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="62"/>
+      <c r="E150" s="61"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="62"/>
+      <c r="E151" s="61"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="62"/>
+      <c r="E152" s="61"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="62"/>
+      <c r="E153" s="61"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="62"/>
+      <c r="E154" s="61"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="62"/>
+      <c r="E155" s="61"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="62"/>
+      <c r="E156" s="61"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="62"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="62"/>
+      <c r="E158" s="61"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="62"/>
+      <c r="E159" s="61"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="62"/>
+      <c r="E160" s="61"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="62"/>
+      <c r="E161" s="61"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="62"/>
+      <c r="E162" s="61"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="62"/>
+      <c r="E163" s="61"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="62"/>
+      <c r="E164" s="61"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="62"/>
+      <c r="E165" s="61"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="62"/>
+      <c r="E166" s="61"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="62"/>
+      <c r="E167" s="61"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="62"/>
+      <c r="E168" s="61"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="62"/>
+      <c r="E169" s="61"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="62"/>
+      <c r="E170" s="61"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="62"/>
+      <c r="E171" s="61"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="62"/>
+      <c r="E172" s="61"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="62"/>
+      <c r="E173" s="61"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="62"/>
+      <c r="E174" s="61"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="62"/>
+      <c r="E175" s="61"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="62"/>
+      <c r="E176" s="61"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="62"/>
+      <c r="E177" s="61"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="62"/>
+      <c r="E178" s="61"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="62"/>
+      <c r="E179" s="61"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="62"/>
+      <c r="E180" s="61"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="62"/>
+      <c r="E181" s="61"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="62"/>
+      <c r="E182" s="61"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="62"/>
+      <c r="E183" s="61"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="62"/>
+      <c r="E184" s="61"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="62"/>
+      <c r="E185" s="61"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="62"/>
+      <c r="E186" s="61"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="62"/>
+      <c r="E187" s="61"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="62"/>
+      <c r="E188" s="61"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="62"/>
+      <c r="E189" s="61"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="62"/>
+      <c r="E190" s="61"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="62"/>
+      <c r="E191" s="61"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="62"/>
+      <c r="E192" s="61"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="62"/>
+      <c r="E193" s="61"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="62"/>
+      <c r="E194" s="61"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="62"/>
+      <c r="E195" s="61"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="62"/>
+      <c r="E196" s="61"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
-      <c r="E197" s="3"/>
+      <c r="E197" s="61"/>
     </row>
     <row r="198" spans="1:5" s="4" customFormat="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
-      <c r="E198" s="3"/>
+      <c r="E198" s="61"/>
     </row>
     <row r="199" spans="1:5" s="4" customFormat="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
-      <c r="E199" s="3"/>
+      <c r="E199" s="61"/>
     </row>
     <row r="200" spans="1:5" s="4" customFormat="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
-      <c r="E200" s="3"/>
+      <c r="E200" s="61"/>
     </row>
     <row r="201" spans="1:5" s="4" customFormat="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
-      <c r="E201" s="3"/>
+      <c r="E201" s="61"/>
     </row>
     <row r="202" spans="1:5" s="4" customFormat="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
-      <c r="E202" s="3"/>
+      <c r="E202" s="61"/>
     </row>
     <row r="203" spans="1:5" s="4" customFormat="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
-      <c r="E203" s="3"/>
+      <c r="E203" s="61"/>
     </row>
     <row r="204" spans="1:5" s="4" customFormat="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
-      <c r="E204" s="3"/>
+      <c r="E204" s="61"/>
     </row>
     <row r="205" spans="1:5" s="4" customFormat="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
-      <c r="E205" s="3"/>
+      <c r="E205" s="61"/>
     </row>
     <row r="206" spans="1:5" s="4" customFormat="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
-      <c r="E206" s="3"/>
+      <c r="E206" s="61"/>
     </row>
     <row r="207" spans="1:5" s="4" customFormat="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
-      <c r="E207" s="3"/>
+      <c r="E207" s="61"/>
     </row>
     <row r="208" spans="1:5" s="4" customFormat="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
-      <c r="E208" s="3"/>
+      <c r="E208" s="61"/>
     </row>
     <row r="209" spans="1:5" s="4" customFormat="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
-      <c r="E209" s="3"/>
+      <c r="E209" s="61"/>
     </row>
     <row r="210" spans="1:5" s="4" customFormat="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
-      <c r="E210" s="3"/>
+      <c r="E210" s="61"/>
     </row>
     <row r="211" spans="1:5" s="4" customFormat="1">
       <c r="A211" s="1"/>
@@ -3421,8 +3561,111 @@
       <c r="D241" s="2"/>
       <c r="E241" s="3"/>
     </row>
+    <row r="242" spans="1:5" s="4" customFormat="1">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="3"/>
+    </row>
+    <row r="243" spans="1:5" s="4" customFormat="1">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="2"/>
+      <c r="E243" s="3"/>
+    </row>
+    <row r="244" spans="1:5" s="4" customFormat="1">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="3"/>
+    </row>
+    <row r="245" spans="1:5" s="4" customFormat="1">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="2"/>
+      <c r="E245" s="3"/>
+    </row>
+    <row r="246" spans="1:5" s="4" customFormat="1">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="2"/>
+      <c r="E246" s="3"/>
+    </row>
+    <row r="247" spans="1:5" s="4" customFormat="1">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="2"/>
+      <c r="E247" s="3"/>
+    </row>
+    <row r="248" spans="1:5" s="4" customFormat="1">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="3"/>
+    </row>
+    <row r="249" spans="1:5" s="4" customFormat="1">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="3"/>
+    </row>
+    <row r="250" spans="1:5" s="4" customFormat="1">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="2"/>
+      <c r="E250" s="3"/>
+    </row>
+    <row r="251" spans="1:5" s="4" customFormat="1">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="2"/>
+      <c r="E251" s="3"/>
+    </row>
+    <row r="252" spans="1:5" s="4" customFormat="1">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="2"/>
+      <c r="E252" s="3"/>
+    </row>
+    <row r="253" spans="1:5" s="4" customFormat="1">
+      <c r="A253" s="1"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="2"/>
+      <c r="E253" s="3"/>
+    </row>
+    <row r="254" spans="1:5" s="4" customFormat="1">
+      <c r="A254" s="1"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="2"/>
+      <c r="E254" s="3"/>
+    </row>
+    <row r="255" spans="1:5" s="4" customFormat="1">
+      <c r="A255" s="1"/>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="2"/>
+      <c r="E255" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3430,13 +3673,8 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(Teleop/hardware): New buttons and functions
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="203">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Change Camera Operator Side</t>
   </si>
   <si>
-    <t>Right 10</t>
-  </si>
-  <si>
-    <t>Right 3</t>
-  </si>
-  <si>
     <t>Change Camera Driver Side</t>
   </si>
   <si>
@@ -468,18 +462,6 @@
     <t>addBallButton</t>
   </si>
   <si>
-    <t>Right 5</t>
-  </si>
-  <si>
-    <t>Right1</t>
-  </si>
-  <si>
-    <t>Right 9</t>
-  </si>
-  <si>
-    <t>Right 8</t>
-  </si>
-  <si>
     <t>Launch Ball</t>
   </si>
   <si>
@@ -565,6 +547,90 @@
   </si>
   <si>
     <t>11/12</t>
+  </si>
+  <si>
+    <t>Drive Delay Timer</t>
+  </si>
+  <si>
+    <t>Launch Delay Timer</t>
+  </si>
+  <si>
+    <t>driveDelayTimer</t>
+  </si>
+  <si>
+    <t>launchDelayTimer</t>
+  </si>
+  <si>
+    <t>climbUpButton</t>
+  </si>
+  <si>
+    <t>Right Operator 3</t>
+  </si>
+  <si>
+    <t>climbDownButton</t>
+  </si>
+  <si>
+    <t>Climb Down Button</t>
+  </si>
+  <si>
+    <t>Climb Up Button</t>
+  </si>
+  <si>
+    <t>Outtake Button</t>
+  </si>
+  <si>
+    <t>outtakeButton</t>
+  </si>
+  <si>
+    <t>Left Operator 2</t>
+  </si>
+  <si>
+    <t>Right Operator 2</t>
+  </si>
+  <si>
+    <t>Ball Counter</t>
+  </si>
+  <si>
+    <t>ballCounter</t>
+  </si>
+  <si>
+    <t>Right Operator 5</t>
+  </si>
+  <si>
+    <t>Right Operator 8</t>
+  </si>
+  <si>
+    <t>Right Operator 9</t>
+  </si>
+  <si>
+    <t>Right Driver 3</t>
+  </si>
+  <si>
+    <t>Right Operator 10</t>
+  </si>
+  <si>
+    <t>Climb Timer</t>
+  </si>
+  <si>
+    <t>climbTimer</t>
+  </si>
+  <si>
+    <t>Close Climb Servo</t>
+  </si>
+  <si>
+    <t>closeClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator 4</t>
+  </si>
+  <si>
+    <t>Open Climb Servo</t>
+  </si>
+  <si>
+    <t>openClimbServo</t>
+  </si>
+  <si>
+    <t>Right Operator Trigger</t>
   </si>
 </sst>
 </file>
@@ -574,7 +640,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,6 +701,14 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF993300"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -736,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -909,9 +983,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,14 +1013,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,7 +1343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,36 +1351,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK241"/>
+  <dimension ref="A1:AMK255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1314,10 +1400,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1329,10 +1415,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>109</v>
+        <v>127</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1342,10 +1428,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>108</v>
+        <v>128</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1355,58 +1441,58 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="22" customFormat="1">
+        <v>129</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
+        <v>130</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="63" t="s">
+      <c r="C9" s="63" t="s">
         <v>159</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>153</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1415,105 +1501,105 @@
       <c r="D10" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="64" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+        <v>96</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+      <c r="C13" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="64" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
+      <c r="C15" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="63" t="s">
+      <c r="C16" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+      <c r="E16" s="62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="66" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+      <c r="C17" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1523,99 +1609,99 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="71"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+      <c r="C20" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+        <v>116</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="63" t="s">
-        <v>122</v>
+      <c r="C22" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>120</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>119</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="66" t="s">
-        <v>137</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>176</v>
+      <c r="C24" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>170</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="65"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1625,7 +1711,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1635,18 +1721,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="70"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1659,7 +1745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1672,88 +1758,88 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
-      <c r="C31" s="64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+      <c r="C31" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
+        <v>133</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
-      <c r="C33" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>179</v>
-      </c>
-      <c r="E33" s="63" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+      <c r="C33" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1791,15 +1877,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="70"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1817,7 +1903,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1914,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1838,10 +1924,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="70"/>
+      <c r="D50" s="68"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1859,41 +1945,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="65" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1903,10 +1989,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="70" t="s">
+      <c r="C57" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="70"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -1924,66 +2010,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="70" t="s">
+      <c r="C62" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="70"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="68" t="s">
-        <v>141</v>
+      <c r="C63" s="67" t="s">
+        <v>139</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="E63" s="63" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
+        <v>138</v>
+      </c>
+      <c r="E63" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -1999,18 +2085,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="70" t="s">
+      <c r="C68" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="70"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2023,14 +2109,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2046,19 +2132,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="70" t="s">
+      <c r="C73" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="70"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2072,7 +2158,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2086,7 +2172,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2100,7 +2186,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2114,13 +2200,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="70" t="s">
+      <c r="C78" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="70"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2133,154 +2219,184 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
-      <c r="C80" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="D80" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" s="63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
+      <c r="C80" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D80" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" s="62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
-      <c r="C82" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D82" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="E82" s="63" t="s">
+      <c r="C82" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="65" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
+      <c r="E82" s="62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D83" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="E83" s="65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1">
+    </row>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
-      <c r="C84" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="D84" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="E84" s="63" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A85" s="5"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="E85" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="F85" s="55"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
+      <c r="C84" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="62" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="75" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A85" s="57"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="F85" s="74"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
-      <c r="C86" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="D86" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="E86" s="63" t="s">
-        <v>151</v>
+      <c r="C86" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" s="62" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E87" s="65" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="E87" s="64" t="s">
+        <v>192</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="16"/>
+      <c r="C88" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88" s="62" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="31"/>
-      <c r="E89" s="56"/>
+      <c r="C89" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="E89" s="56" t="s">
+        <v>187</v>
+      </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="16"/>
+      <c r="C90" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="D90" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="E90" s="62" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="20"/>
+      <c r="C91" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" s="64" t="s">
+        <v>199</v>
+      </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="16"/>
+      <c r="C92" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="D92" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E92" s="62" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
@@ -2290,7 +2406,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2320,26 +2436,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="70" t="s">
+      <c r="C99" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="70"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2352,38 +2468,38 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="58"/>
       <c r="E102" s="38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D103" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="E103" s="65" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
+        <v>168</v>
+      </c>
+      <c r="E103" s="64" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2396,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2405,11 +2521,11 @@
       <c r="D105" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E105" s="60" t="s">
+      <c r="E105" s="59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2418,24 +2534,24 @@
       <c r="D106" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E106" s="61" t="s">
+      <c r="E106" s="60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E107" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2448,7 +2564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2461,7 +2577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2474,20 +2590,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2500,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2513,696 +2629,720 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="29"/>
-      <c r="E114" s="16"/>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E115" s="30" t="s">
+      <c r="C114" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D114" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A115" s="17"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E115" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
-      <c r="C116" s="28" t="s">
+      <c r="C116" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="D116" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="E116" s="62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="D117" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E117" s="64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="16"/>
+    </row>
+    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A119" s="17"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="41"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="20"/>
+    </row>
+    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="29"/>
+      <c r="E120" s="16"/>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="41"/>
+      <c r="D121" s="42"/>
+      <c r="E121" s="20"/>
+    </row>
+    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="16"/>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A123" s="17"/>
+      <c r="B123" s="17"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="42"/>
+      <c r="E123" s="20"/>
+    </row>
+    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="16"/>
+    </row>
+    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A125" s="17"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="41"/>
+      <c r="D125" s="42"/>
+      <c r="E125" s="20"/>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="29"/>
+      <c r="E126" s="16"/>
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A127" s="17"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="42"/>
+      <c r="E127" s="20"/>
+    </row>
+    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="16"/>
+    </row>
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D116" s="29" t="s">
+      <c r="D130" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="E130" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="62"/>
-    </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="62"/>
-    </row>
-    <row r="119" spans="1:5" s="4" customFormat="1">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="62"/>
-    </row>
-    <row r="120" spans="1:5" s="4" customFormat="1">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="62"/>
-    </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="62"/>
-    </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="62"/>
-    </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="62"/>
-    </row>
-    <row r="124" spans="1:5" s="4" customFormat="1">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="62"/>
-    </row>
-    <row r="125" spans="1:5" s="4" customFormat="1">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="62"/>
-    </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="62"/>
-    </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="62"/>
-    </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="62"/>
-    </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="62"/>
-    </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="62"/>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="2"/>
-      <c r="E131" s="62"/>
+      <c r="E131" s="61"/>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="62"/>
+      <c r="E132" s="61"/>
     </row>
     <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="62"/>
+      <c r="E133" s="61"/>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="62"/>
+      <c r="E134" s="61"/>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="62"/>
+      <c r="E135" s="61"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="62"/>
+      <c r="E136" s="61"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="62"/>
+      <c r="E137" s="61"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="62"/>
+      <c r="E138" s="61"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="62"/>
+      <c r="E139" s="61"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="62"/>
+      <c r="E140" s="61"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="62"/>
+      <c r="E141" s="61"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="62"/>
+      <c r="E142" s="61"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="62"/>
+      <c r="E143" s="61"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="62"/>
+      <c r="E144" s="61"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="62"/>
+      <c r="E145" s="61"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="62"/>
+      <c r="E146" s="61"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="62"/>
+      <c r="E147" s="61"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="62"/>
+      <c r="E148" s="61"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="62"/>
+      <c r="E149" s="61"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="62"/>
+      <c r="E150" s="61"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="62"/>
+      <c r="E151" s="61"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="62"/>
+      <c r="E152" s="61"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="62"/>
+      <c r="E153" s="61"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="62"/>
+      <c r="E154" s="61"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="62"/>
+      <c r="E155" s="61"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="62"/>
+      <c r="E156" s="61"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="62"/>
+      <c r="E157" s="61"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="62"/>
+      <c r="E158" s="61"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="62"/>
+      <c r="E159" s="61"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="62"/>
+      <c r="E160" s="61"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="62"/>
+      <c r="E161" s="61"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="62"/>
+      <c r="E162" s="61"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="62"/>
+      <c r="E163" s="61"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="62"/>
+      <c r="E164" s="61"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="62"/>
+      <c r="E165" s="61"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="62"/>
+      <c r="E166" s="61"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="62"/>
+      <c r="E167" s="61"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="62"/>
+      <c r="E168" s="61"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="62"/>
+      <c r="E169" s="61"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="62"/>
+      <c r="E170" s="61"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="62"/>
+      <c r="E171" s="61"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="62"/>
+      <c r="E172" s="61"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="62"/>
+      <c r="E173" s="61"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="62"/>
+      <c r="E174" s="61"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="62"/>
+      <c r="E175" s="61"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="62"/>
+      <c r="E176" s="61"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="62"/>
+      <c r="E177" s="61"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="62"/>
+      <c r="E178" s="61"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="62"/>
+      <c r="E179" s="61"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="62"/>
+      <c r="E180" s="61"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="62"/>
+      <c r="E181" s="61"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="62"/>
+      <c r="E182" s="61"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="62"/>
+      <c r="E183" s="61"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="62"/>
+      <c r="E184" s="61"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="62"/>
+      <c r="E185" s="61"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="62"/>
+      <c r="E186" s="61"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="62"/>
+      <c r="E187" s="61"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="62"/>
+      <c r="E188" s="61"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="62"/>
+      <c r="E189" s="61"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="62"/>
+      <c r="E190" s="61"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="62"/>
+      <c r="E191" s="61"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="62"/>
+      <c r="E192" s="61"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="62"/>
+      <c r="E193" s="61"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="62"/>
+      <c r="E194" s="61"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="62"/>
+      <c r="E195" s="61"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="62"/>
+      <c r="E196" s="61"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
-      <c r="E197" s="3"/>
+      <c r="E197" s="61"/>
     </row>
     <row r="198" spans="1:5" s="4" customFormat="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
-      <c r="E198" s="3"/>
+      <c r="E198" s="61"/>
     </row>
     <row r="199" spans="1:5" s="4" customFormat="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
-      <c r="E199" s="3"/>
+      <c r="E199" s="61"/>
     </row>
     <row r="200" spans="1:5" s="4" customFormat="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
-      <c r="E200" s="3"/>
+      <c r="E200" s="61"/>
     </row>
     <row r="201" spans="1:5" s="4" customFormat="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
-      <c r="E201" s="3"/>
+      <c r="E201" s="61"/>
     </row>
     <row r="202" spans="1:5" s="4" customFormat="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
-      <c r="E202" s="3"/>
+      <c r="E202" s="61"/>
     </row>
     <row r="203" spans="1:5" s="4" customFormat="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
-      <c r="E203" s="3"/>
+      <c r="E203" s="61"/>
     </row>
     <row r="204" spans="1:5" s="4" customFormat="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
-      <c r="E204" s="3"/>
+      <c r="E204" s="61"/>
     </row>
     <row r="205" spans="1:5" s="4" customFormat="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
-      <c r="E205" s="3"/>
+      <c r="E205" s="61"/>
     </row>
     <row r="206" spans="1:5" s="4" customFormat="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
-      <c r="E206" s="3"/>
+      <c r="E206" s="61"/>
     </row>
     <row r="207" spans="1:5" s="4" customFormat="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
-      <c r="E207" s="3"/>
+      <c r="E207" s="61"/>
     </row>
     <row r="208" spans="1:5" s="4" customFormat="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
-      <c r="E208" s="3"/>
+      <c r="E208" s="61"/>
     </row>
     <row r="209" spans="1:5" s="4" customFormat="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
-      <c r="E209" s="3"/>
+      <c r="E209" s="61"/>
     </row>
     <row r="210" spans="1:5" s="4" customFormat="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
-      <c r="E210" s="3"/>
+      <c r="E210" s="61"/>
     </row>
     <row r="211" spans="1:5" s="4" customFormat="1">
       <c r="A211" s="1"/>
@@ -3421,8 +3561,111 @@
       <c r="D241" s="2"/>
       <c r="E241" s="3"/>
     </row>
+    <row r="242" spans="1:5" s="4" customFormat="1">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="3"/>
+    </row>
+    <row r="243" spans="1:5" s="4" customFormat="1">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="2"/>
+      <c r="E243" s="3"/>
+    </row>
+    <row r="244" spans="1:5" s="4" customFormat="1">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="3"/>
+    </row>
+    <row r="245" spans="1:5" s="4" customFormat="1">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="2"/>
+      <c r="E245" s="3"/>
+    </row>
+    <row r="246" spans="1:5" s="4" customFormat="1">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
+      <c r="D246" s="2"/>
+      <c r="E246" s="3"/>
+    </row>
+    <row r="247" spans="1:5" s="4" customFormat="1">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
+      <c r="D247" s="2"/>
+      <c r="E247" s="3"/>
+    </row>
+    <row r="248" spans="1:5" s="4" customFormat="1">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="3"/>
+    </row>
+    <row r="249" spans="1:5" s="4" customFormat="1">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="3"/>
+    </row>
+    <row r="250" spans="1:5" s="4" customFormat="1">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="2"/>
+      <c r="E250" s="3"/>
+    </row>
+    <row r="251" spans="1:5" s="4" customFormat="1">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="2"/>
+      <c r="E251" s="3"/>
+    </row>
+    <row r="252" spans="1:5" s="4" customFormat="1">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="2"/>
+      <c r="E252" s="3"/>
+    </row>
+    <row r="253" spans="1:5" s="4" customFormat="1">
+      <c r="A253" s="1"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="2"/>
+      <c r="E253" s="3"/>
+    </row>
+    <row r="254" spans="1:5" s="4" customFormat="1">
+      <c r="A254" s="1"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+      <c r="D254" s="2"/>
+      <c r="E254" s="3"/>
+    </row>
+    <row r="255" spans="1:5" s="4" customFormat="1">
+      <c r="A255" s="1"/>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="2"/>
+      <c r="E255" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3430,13 +3673,8 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to equipment list
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -429,9 +429,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>floorLight</t>
-  </si>
-  <si>
     <t>Spin Switch</t>
   </si>
   <si>
@@ -474,9 +471,6 @@
     <t>Add to Ball Count</t>
   </si>
   <si>
-    <t>Floor Light</t>
-  </si>
-  <si>
     <t>launchMotorForward</t>
   </si>
   <si>
@@ -534,9 +528,6 @@
     <t>tankTransmission</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -631,6 +622,15 @@
   </si>
   <si>
     <t>Right Operator Trigger</t>
+  </si>
+  <si>
+    <t>Fire Override</t>
+  </si>
+  <si>
+    <t>fireOverride</t>
+  </si>
+  <si>
+    <t>Left Operator 11</t>
   </si>
 </sst>
 </file>
@@ -1013,6 +1013,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1021,21 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,33 +1354,33 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1400,10 +1400,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
@@ -1460,39 +1460,39 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1508,7 +1508,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="63" t="s">
@@ -1521,7 +1521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1534,7 +1534,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="63" t="s">
@@ -1547,7 +1547,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1560,20 +1560,20 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="63" t="s">
@@ -1586,20 +1586,20 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E17" s="62" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1609,15 +1609,15 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="75"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="63" t="s">
@@ -1630,7 +1630,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
@@ -1643,7 +1643,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="63" t="s">
@@ -1659,7 +1659,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
@@ -1675,23 +1675,17 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="62" t="s">
-        <v>170</v>
-      </c>
+      <c r="C24" s="63"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="62"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1701,7 +1695,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1711,7 +1705,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1721,18 +1715,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1745,7 +1739,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1758,11 +1752,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="65" t="s">
         <v>131</v>
@@ -1771,11 +1765,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="32" spans="1:8" s="4" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>133</v>
@@ -1784,62 +1778,62 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="63" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D33" s="65" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1877,15 +1871,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="73"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1903,7 +1897,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1914,7 +1908,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1924,10 +1918,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="73"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1945,41 +1939,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1989,10 +1983,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="73"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -2010,66 +2004,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
       <c r="C63" s="67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E63" s="62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -2085,18 +2079,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="73"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2109,14 +2103,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2132,19 +2126,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="73"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2158,7 +2152,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2172,7 +2166,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2186,7 +2180,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2200,13 +2194,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2219,10 +2213,10 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
@@ -2232,13 +2226,13 @@
         <v>89</v>
       </c>
       <c r="D80" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E80" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
@@ -2251,7 +2245,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="62" t="s">
@@ -2264,7 +2258,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
@@ -2281,132 +2275,138 @@
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="63" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D84" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E84" s="62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="75" customFormat="1" ht="13.15" customHeight="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="72" customFormat="1" ht="13.15" customHeight="1">
       <c r="A85" s="57"/>
       <c r="B85" s="57"/>
-      <c r="C85" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="D85" s="72" t="s">
-        <v>143</v>
-      </c>
-      <c r="E85" s="73" t="s">
-        <v>190</v>
-      </c>
-      <c r="F85" s="74"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="C85" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D85" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="F85" s="71"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D86" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E86" s="62" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E87" s="64" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D88" s="65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E88" s="62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
       <c r="C89" s="32" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E89" s="56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D90" s="65" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E90" s="62" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
       <c r="C91" s="32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E91" s="64" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="63" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D92" s="65" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E92" s="62" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="17"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="20"/>
+      <c r="C93" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D93" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="E93" s="64" t="s">
+        <v>202</v>
+      </c>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2436,26 +2436,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="73"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2468,14 +2468,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2486,20 +2486,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D103" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E103" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="E103" s="64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2512,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2525,7 +2525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2538,20 +2538,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2564,7 +2564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2577,7 +2577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2590,20 +2590,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2616,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2629,136 +2629,136 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="63" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D114" s="65" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E115" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D116" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E116" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D117" s="33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E117" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
       <c r="C118" s="28"/>
       <c r="D118" s="29"/>
       <c r="E118" s="16"/>
     </row>
-    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="119" spans="1:5" s="4" customFormat="1">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="41"/>
       <c r="D119" s="42"/>
       <c r="E119" s="20"/>
     </row>
-    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="120" spans="1:5" s="4" customFormat="1">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
       <c r="C120" s="28"/>
       <c r="D120" s="29"/>
       <c r="E120" s="16"/>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="41"/>
       <c r="D121" s="42"/>
       <c r="E121" s="20"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="21"/>
       <c r="B122" s="21"/>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
       <c r="E122" s="16"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="41"/>
       <c r="D123" s="42"/>
       <c r="E123" s="20"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="21"/>
       <c r="B124" s="21"/>
       <c r="C124" s="28"/>
       <c r="D124" s="29"/>
       <c r="E124" s="16"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="C125" s="41"/>
       <c r="D125" s="42"/>
       <c r="E125" s="20"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="21"/>
       <c r="B126" s="21"/>
       <c r="C126" s="28"/>
       <c r="D126" s="29"/>
       <c r="E126" s="16"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="C127" s="41"/>
       <c r="D127" s="42"/>
       <c r="E127" s="20"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="21"/>
       <c r="B128" s="21"/>
       <c r="C128" s="28"/>
       <c r="D128" s="29"/>
       <c r="E128" s="16"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="30" t="s">
@@ -2771,7 +2771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
       <c r="C130" s="28" t="s">

</xml_diff>

<commit_message>
removed unused sensors and floor light
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -429,9 +429,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>floorLight</t>
-  </si>
-  <si>
     <t>Spin Switch</t>
   </si>
   <si>
@@ -474,9 +471,6 @@
     <t>Add to Ball Count</t>
   </si>
   <si>
-    <t>Floor Light</t>
-  </si>
-  <si>
     <t>launchMotorForward</t>
   </si>
   <si>
@@ -534,9 +528,6 @@
     <t>tankTransmission</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -631,6 +622,15 @@
   </si>
   <si>
     <t>Right Operator Trigger</t>
+  </si>
+  <si>
+    <t>Fire Override</t>
+  </si>
+  <si>
+    <t>fireOverride</t>
+  </si>
+  <si>
+    <t>Left Operator 11</t>
   </si>
 </sst>
 </file>
@@ -1013,6 +1013,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1021,21 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,33 +1354,33 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="74" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1400,10 +1400,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
@@ -1460,39 +1460,39 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1508,7 +1508,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="63" t="s">
@@ -1521,7 +1521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1534,7 +1534,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="63" t="s">
@@ -1547,7 +1547,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1560,20 +1560,20 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="63" t="s">
@@ -1586,20 +1586,20 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E17" s="62" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1609,15 +1609,15 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="75"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="63" t="s">
@@ -1630,7 +1630,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
@@ -1643,7 +1643,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="63" t="s">
@@ -1659,7 +1659,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
@@ -1675,23 +1675,17 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
-      <c r="C24" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="62" t="s">
-        <v>170</v>
-      </c>
+      <c r="C24" s="63"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="62"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1701,7 +1695,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1711,7 +1705,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1721,18 +1715,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1745,7 +1739,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1758,11 +1752,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D31" s="65" t="s">
         <v>131</v>
@@ -1771,11 +1765,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="32" spans="1:8" s="4" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>133</v>
@@ -1784,62 +1778,62 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="63" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D33" s="65" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E33" s="62" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1877,15 +1871,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="73"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1903,7 +1897,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1914,7 +1908,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="49" spans="1:5" s="4" customFormat="1">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1924,10 +1918,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="73"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1945,41 +1939,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E52" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="54" spans="1:5" s="4" customFormat="1">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="55" spans="1:5" s="4" customFormat="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1989,10 +1983,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="73"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -2010,66 +2004,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="61" spans="1:5" s="4" customFormat="1">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
       <c r="C63" s="67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E63" s="62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="66" spans="1:8" s="4" customFormat="1">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -2085,18 +2079,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="73"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2109,14 +2103,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="71" spans="1:8" s="4" customFormat="1">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2132,19 +2126,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="73"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2158,7 +2152,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2172,7 +2166,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="76" spans="1:8" s="4" customFormat="1">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2186,7 +2180,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="77" spans="1:8" s="4" customFormat="1">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2200,13 +2194,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2219,10 +2213,10 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
@@ -2232,13 +2226,13 @@
         <v>89</v>
       </c>
       <c r="D80" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E80" s="62" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
@@ -2251,7 +2245,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="62" t="s">
@@ -2264,7 +2258,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
@@ -2281,132 +2275,138 @@
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="63" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D84" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E84" s="62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="75" customFormat="1" ht="13.15" customHeight="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="72" customFormat="1" ht="13.15" customHeight="1">
       <c r="A85" s="57"/>
       <c r="B85" s="57"/>
-      <c r="C85" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="D85" s="72" t="s">
-        <v>143</v>
-      </c>
-      <c r="E85" s="73" t="s">
-        <v>190</v>
-      </c>
-      <c r="F85" s="74"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="C85" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D85" s="69" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="F85" s="71"/>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D86" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E86" s="62" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E87" s="64" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="88" spans="1:6" s="4" customFormat="1">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D88" s="65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E88" s="62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
       <c r="C89" s="32" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E89" s="56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:6" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D90" s="65" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E90" s="62" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
       <c r="C91" s="32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E91" s="64" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:6" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="63" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D92" s="65" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E92" s="62" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="17"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="20"/>
+      <c r="C93" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D93" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="E93" s="64" t="s">
+        <v>202</v>
+      </c>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:6" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="28"/>
@@ -2436,26 +2436,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="73"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="100" spans="1:7" s="4" customFormat="1">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2468,14 +2468,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="101" spans="1:7" s="4" customFormat="1">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2486,20 +2486,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="103" spans="1:7" s="4" customFormat="1">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D103" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E103" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="E103" s="64" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2512,7 +2512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2525,7 +2525,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2538,20 +2538,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2564,7 +2564,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2577,7 +2577,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2590,20 +2590,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2616,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2629,136 +2629,136 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="63" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D114" s="65" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E115" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D116" s="65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E116" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D117" s="33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E117" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
       <c r="C118" s="28"/>
       <c r="D118" s="29"/>
       <c r="E118" s="16"/>
     </row>
-    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="119" spans="1:5" s="4" customFormat="1">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="41"/>
       <c r="D119" s="42"/>
       <c r="E119" s="20"/>
     </row>
-    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="120" spans="1:5" s="4" customFormat="1">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
       <c r="C120" s="28"/>
       <c r="D120" s="29"/>
       <c r="E120" s="16"/>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="41"/>
       <c r="D121" s="42"/>
       <c r="E121" s="20"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="21"/>
       <c r="B122" s="21"/>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
       <c r="E122" s="16"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="41"/>
       <c r="D123" s="42"/>
       <c r="E123" s="20"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="21"/>
       <c r="B124" s="21"/>
       <c r="C124" s="28"/>
       <c r="D124" s="29"/>
       <c r="E124" s="16"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="C125" s="41"/>
       <c r="D125" s="42"/>
       <c r="E125" s="20"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="21"/>
       <c r="B126" s="21"/>
       <c r="C126" s="28"/>
       <c r="D126" s="29"/>
       <c r="E126" s="16"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="C127" s="41"/>
       <c r="D127" s="42"/>
       <c r="E127" s="20"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="21"/>
       <c r="B128" s="21"/>
       <c r="C128" s="28"/>
       <c r="D128" s="29"/>
       <c r="E128" s="16"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="30" t="s">
@@ -2771,7 +2771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
       <c r="C130" s="28" t="s">

</xml_diff>

<commit_message>
Fixed intake to work how we want it to and worked on giving launch two settings
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="207">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -333,9 +333,6 @@
     <t>driverGearDownPressed</t>
   </si>
   <si>
-    <t>Left Drivers Gear Up</t>
-  </si>
-  <si>
     <t>CAN 12</t>
   </si>
   <si>
@@ -631,6 +628,21 @@
   </si>
   <si>
     <t>Left Operator 11</t>
+  </si>
+  <si>
+    <t>Left Operator 4</t>
+  </si>
+  <si>
+    <t>Left Operator 5</t>
+  </si>
+  <si>
+    <t>Fire High</t>
+  </si>
+  <si>
+    <t>fireHigh</t>
+  </si>
+  <si>
+    <t>Left Drivers Gear Down</t>
   </si>
 </sst>
 </file>
@@ -810,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1026,6 +1038,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1354,33 +1369,33 @@
   <dimension ref="A1:AMK255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1"/>
+    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="74" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
+      <c r="A1" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1400,10 +1415,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1415,10 +1430,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1428,10 +1443,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1441,58 +1456,58 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E6" s="64" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="22" customFormat="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="62" t="s">
         <v>150</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>151</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
@@ -1508,7 +1523,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="63" t="s">
@@ -1521,7 +1536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="32" t="s">
@@ -1534,7 +1549,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="63" t="s">
@@ -1547,33 +1562,33 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="E14" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="E15" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="E15" s="62" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="63" t="s">
@@ -1586,20 +1601,20 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1">
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="35"/>
@@ -1609,73 +1624,73 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="75"/>
+      <c r="D19" s="76"/>
       <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="65" t="s">
-        <v>115</v>
-      </c>
       <c r="E20" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A21" s="39"/>
       <c r="B21" s="39"/>
       <c r="C21" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="64" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="64" t="s">
         <v>118</v>
-      </c>
-      <c r="E23" s="64" t="s">
-        <v>119</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
       <c r="C24" s="63"/>
@@ -1685,7 +1700,7 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
       <c r="C25" s="32"/>
@@ -1695,7 +1710,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="28"/>
@@ -1705,7 +1720,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="41"/>
@@ -1715,18 +1730,18 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="73"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="28" t="s">
@@ -1739,7 +1754,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="30" t="s">
@@ -1752,88 +1767,88 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D31" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="62" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1">
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D32" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="64" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1">
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="65" t="s">
+      <c r="E33" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="E33" s="62" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1">
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="20"/>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1">
+    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="28"/>
       <c r="D35" s="43"/>
       <c r="E35" s="16"/>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="28"/>
       <c r="D37" s="29"/>
       <c r="E37" s="16"/>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="32"/>
       <c r="D38" s="44"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
@@ -1871,15 +1886,15 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="37"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="73"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1">
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A46" s="46" t="s">
         <v>25</v>
       </c>
@@ -1897,7 +1912,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="30"/>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1">
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A48" s="21" t="s">
         <v>25</v>
       </c>
@@ -1908,7 +1923,7 @@
       <c r="D48" s="29"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1">
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="41"/>
@@ -1918,10 +1933,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="37"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="73"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="9" t="s">
         <v>27</v>
       </c>
@@ -1939,41 +1954,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="32" t="s">
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A52" s="57"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="64" t="s">
+      <c r="E52" s="70" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1">
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="28"/>
       <c r="D53" s="29"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1">
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="32"/>
       <c r="D54" s="33"/>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1">
+    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1">
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="32"/>
@@ -1983,10 +1998,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="37"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="73"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
@@ -2004,66 +2019,66 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1">
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="41"/>
       <c r="D59" s="33"/>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1">
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1">
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="32"/>
       <c r="D61" s="33"/>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A62" s="37"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1">
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A63" s="51"/>
       <c r="B63" s="51"/>
       <c r="C63" s="67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E63" s="62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="32"/>
       <c r="D64" s="33"/>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1">
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="32"/>
@@ -2079,18 +2094,18 @@
       <c r="G67" s="54"/>
       <c r="H67" s="54"/>
     </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A68" s="37"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="73" t="s">
+      <c r="C68" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="73"/>
+      <c r="D68" s="74"/>
       <c r="E68" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1">
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="41" t="s">
@@ -2103,14 +2118,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1">
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="28"/>
       <c r="D70" s="29"/>
       <c r="E70" s="16"/>
     </row>
-    <row r="71" spans="1:8" s="4" customFormat="1">
+    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="41"/>
@@ -2126,19 +2141,19 @@
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A73" s="37"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="73" t="s">
+      <c r="C73" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="73"/>
+      <c r="D73" s="74"/>
       <c r="E73" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G73" s="55"/>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1">
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="32" t="s">
@@ -2152,7 +2167,7 @@
       </c>
       <c r="G74" s="55"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1">
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="28" t="s">
@@ -2166,7 +2181,7 @@
       </c>
       <c r="G75" s="55"/>
     </row>
-    <row r="76" spans="1:8" s="4" customFormat="1">
+    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="30" t="s">
@@ -2180,7 +2195,7 @@
       </c>
       <c r="G76" s="55"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="28" t="s">
@@ -2194,13 +2209,13 @@
       </c>
       <c r="G77" s="55"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A78" s="37"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="73" t="s">
+      <c r="C78" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="D78" s="73"/>
+      <c r="D78" s="74"/>
       <c r="E78" s="9" t="s">
         <v>54</v>
       </c>
@@ -2213,10 +2228,10 @@
         <v>88</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
@@ -2226,17 +2241,17 @@
         <v>89</v>
       </c>
       <c r="D80" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E80" s="62" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="32" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="D81" s="32" t="s">
         <v>102</v>
@@ -2245,7 +2260,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1">
+    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="62" t="s">
@@ -2258,160 +2273,166 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25.5">
+    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
       <c r="A83" s="42"/>
       <c r="B83" s="42"/>
       <c r="C83" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D83" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="D83" s="33" t="s">
+      <c r="E83" s="64" t="s">
         <v>125</v>
-      </c>
-      <c r="E83" s="64" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="4" customFormat="1" ht="25.5">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D84" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E84" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="72" customFormat="1" ht="13.15" customHeight="1">
       <c r="A85" s="57"/>
       <c r="B85" s="57"/>
       <c r="C85" s="68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D85" s="69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E85" s="70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F85" s="71"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1">
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D86" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E86" s="62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A87" s="5"/>
       <c r="B87" s="17"/>
       <c r="C87" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E87" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F87" s="55"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1">
+    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D88" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" s="62" t="s">
         <v>176</v>
-      </c>
-      <c r="E88" s="62" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" s="17"/>
       <c r="C89" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E89" s="56" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F89" s="55"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1">
+    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D90" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="D90" s="65" t="s">
+      <c r="E90" s="62" t="s">
         <v>182</v>
-      </c>
-      <c r="E90" s="62" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
       <c r="C91" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D91" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="D91" s="33" t="s">
-        <v>195</v>
-      </c>
       <c r="E91" s="64" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F91" s="55"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1">
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="D92" s="65" t="s">
         <v>197</v>
       </c>
-      <c r="D92" s="65" t="s">
-        <v>198</v>
-      </c>
       <c r="E92" s="62" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="17"/>
       <c r="C93" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="D93" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D93" s="33" t="s">
+      <c r="E93" s="64" t="s">
         <v>201</v>
       </c>
-      <c r="E93" s="64" t="s">
-        <v>202</v>
-      </c>
       <c r="F93" s="55"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1">
+    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="16"/>
+      <c r="C94" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="D94" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="E94" s="62" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="95" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A95" s="5"/>
@@ -2436,26 +2457,26 @@
       <c r="E97" s="20"/>
       <c r="F97" s="55"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1">
+    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="28"/>
       <c r="D98" s="29"/>
       <c r="E98" s="16"/>
     </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A99" s="37"/>
       <c r="B99" s="37"/>
-      <c r="C99" s="73" t="s">
+      <c r="C99" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="D99" s="73"/>
+      <c r="D99" s="74"/>
       <c r="E99" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G99" s="55"/>
     </row>
-    <row r="100" spans="1:7" s="4" customFormat="1">
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="56" t="s">
@@ -2468,14 +2489,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="4" customFormat="1">
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="28"/>
       <c r="D101" s="29"/>
       <c r="E101" s="16"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1">
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A102" s="37"/>
       <c r="B102" s="37"/>
       <c r="C102" s="38" t="s">
@@ -2486,20 +2507,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D103" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="D103" s="33" t="s">
-        <v>166</v>
-      </c>
       <c r="E103" s="64" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="28" t="s">
@@ -2512,7 +2533,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1">
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="41" t="s">
@@ -2525,7 +2546,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1">
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
@@ -2538,20 +2559,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1">
+    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E107" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="4" customFormat="1">
+    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
@@ -2564,7 +2585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1">
+    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="30" t="s">
@@ -2577,7 +2598,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1">
+    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2590,20 +2611,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1">
+    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E111" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1">
+    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2616,7 +2637,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2629,136 +2650,136 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D114" s="65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E114" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1">
+    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E115" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="D116" s="65" t="s">
         <v>185</v>
-      </c>
-      <c r="D116" s="65" t="s">
-        <v>186</v>
       </c>
       <c r="E116" s="62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
+    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="D117" s="33" t="s">
         <v>192</v>
-      </c>
-      <c r="D117" s="33" t="s">
-        <v>193</v>
       </c>
       <c r="E117" s="64" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
+    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
       <c r="C118" s="28"/>
       <c r="D118" s="29"/>
       <c r="E118" s="16"/>
     </row>
-    <row r="119" spans="1:5" s="4" customFormat="1">
+    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="41"/>
       <c r="D119" s="42"/>
       <c r="E119" s="20"/>
     </row>
-    <row r="120" spans="1:5" s="4" customFormat="1">
+    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
       <c r="C120" s="28"/>
       <c r="D120" s="29"/>
       <c r="E120" s="16"/>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
+    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="41"/>
       <c r="D121" s="42"/>
       <c r="E121" s="20"/>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
+    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A122" s="21"/>
       <c r="B122" s="21"/>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
       <c r="E122" s="16"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
+    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="41"/>
       <c r="D123" s="42"/>
       <c r="E123" s="20"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1">
+    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A124" s="21"/>
       <c r="B124" s="21"/>
       <c r="C124" s="28"/>
       <c r="D124" s="29"/>
       <c r="E124" s="16"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1">
+    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="C125" s="41"/>
       <c r="D125" s="42"/>
       <c r="E125" s="20"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
+    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A126" s="21"/>
       <c r="B126" s="21"/>
       <c r="C126" s="28"/>
       <c r="D126" s="29"/>
       <c r="E126" s="16"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
+    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="C127" s="41"/>
       <c r="D127" s="42"/>
       <c r="E127" s="20"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
+    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A128" s="21"/>
       <c r="B128" s="21"/>
       <c r="C128" s="28"/>
       <c r="D128" s="29"/>
       <c r="E128" s="16"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
+    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="30" t="s">
@@ -2771,7 +2792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
+    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
       <c r="C130" s="28" t="s">

</xml_diff>

<commit_message>
Fixed launcher to work with 2022
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$101</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$105</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="220">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -57,18 +57,6 @@
     <t>Right Rear Motor (controller_type)</t>
   </si>
   <si>
-    <t>Left Drive Encoder</t>
-  </si>
-  <si>
-    <t>(leftFrontMotor)</t>
-  </si>
-  <si>
-    <t>Right Drive Encoder</t>
-  </si>
-  <si>
-    <t>(rightFrontMotor)</t>
-  </si>
-  <si>
     <t>IR Sensor/Red Light Sensors (see also Digital Inputs)</t>
   </si>
   <si>
@@ -204,9 +192,6 @@
     <t>IP Address</t>
   </si>
   <si>
-    <t>Classmate/Toshiba</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -276,12 +261,6 @@
     <t>drive</t>
   </si>
   <si>
-    <t>leftDriveEncoder</t>
-  </si>
-  <si>
-    <t>rightDriveEncoder</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -495,12 +474,6 @@
     <t>Launch Motor Backward</t>
   </si>
   <si>
-    <t>colorWheelMotor</t>
-  </si>
-  <si>
-    <t>Color Wheel Motor</t>
-  </si>
-  <si>
     <t>5, 4</t>
   </si>
   <si>
@@ -643,6 +616,72 @@
   </si>
   <si>
     <t>Left Drivers Gear Down</t>
+  </si>
+  <si>
+    <t>leftDriveTopEncoder</t>
+  </si>
+  <si>
+    <t>rightDriveTopEncoder</t>
+  </si>
+  <si>
+    <t>Left Drive Top Encoder</t>
+  </si>
+  <si>
+    <t>Right Drive Top Encoder</t>
+  </si>
+  <si>
+    <t>Left Drive Bottom Encoder</t>
+  </si>
+  <si>
+    <t>Right Drive Bottom Encoder</t>
+  </si>
+  <si>
+    <t>leftDriveBottomEncoder</t>
+  </si>
+  <si>
+    <t>rightDriveBottomEncoder</t>
+  </si>
+  <si>
+    <t>(leftFrontTopMotor)</t>
+  </si>
+  <si>
+    <t>(rightFrontTopMotor)</t>
+  </si>
+  <si>
+    <t>(leftFrontBottomMotor)</t>
+  </si>
+  <si>
+    <t>(rightFrontBottomMotor)</t>
+  </si>
+  <si>
+    <t>Launcher Motor Encoder</t>
+  </si>
+  <si>
+    <t>launchMotorEncoder</t>
+  </si>
+  <si>
+    <t>launcherMotor</t>
+  </si>
+  <si>
+    <t>Conveyor Motor Forward</t>
+  </si>
+  <si>
+    <t>conveyorMotorForward</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Conveyor Motor Backward</t>
+  </si>
+  <si>
+    <t>conveyorMotorBackward</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Classmate/Toshiba DriverStation</t>
   </si>
 </sst>
 </file>
@@ -822,7 +861,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -923,15 +962,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1043,14 +1073,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,7 +1391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1366,11 +1399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK255"/>
+  <dimension ref="A1:AMK259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -1387,13 +1420,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
+      <c r="A1" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
       <c r="A2" s="5" t="s">
@@ -1415,10 +1448,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="72"/>
       <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1430,10 +1463,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="64" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1443,10 +1476,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>105</v>
+        <v>120</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
@@ -1456,10 +1489,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>104</v>
+        <v>121</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
@@ -1469,23 +1502,23 @@
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>103</v>
+        <v>122</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
@@ -1494,14 +1527,14 @@
     <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="65" t="s">
+      <c r="C9" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="62" t="s">
-        <v>150</v>
+      <c r="D9" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>143</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
@@ -1511,13 +1544,13 @@
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>12</v>
+        <v>198</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>206</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
@@ -1526,196 +1559,205 @@
     <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="C11" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="25.5">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="32" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="13">
+        <v>204</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>94</v>
+      <c r="C13" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>109</v>
+        <v>89</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="63" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" s="62" t="s">
-        <v>154</v>
+      <c r="C15" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>93</v>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>157</v>
-      </c>
-      <c r="E17" s="62" t="s">
-        <v>133</v>
+      <c r="C17" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="34"/>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="76" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="38" t="s">
-        <v>16</v>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="63" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="63"/>
+    </row>
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="73"/>
+      <c r="E23" s="35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="64" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="63" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="16"/>
+      <c r="C26" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>112</v>
+      </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
@@ -1723,1012 +1765,1030 @@
     <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="12"/>
+      <c r="C27" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>111</v>
+      </c>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="13">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>87</v>
-      </c>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="64" t="s">
-        <v>133</v>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="72"/>
+      <c r="E32" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="63" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" s="62" t="s">
-        <v>170</v>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="20"/>
+      <c r="C34" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="16"/>
+      <c r="C35" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="59" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="20"/>
+      <c r="C36" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="61" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="16"/>
+      <c r="C37" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="59" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="12"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="20"/>
     </row>
     <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="40" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
       <c r="E40" s="20"/>
     </row>
-    <row r="41" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+    <row r="41" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+    <row r="42" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="41"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+    <row r="43" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="28"/>
       <c r="D43" s="29"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
+    <row r="44" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="30"/>
       <c r="D44" s="31"/>
       <c r="E44" s="20"/>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="74" t="s">
+    <row r="45" spans="1:5" s="42" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5" s="42" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="1:5" s="42" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="20"/>
+    </row>
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="72"/>
+      <c r="E49" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A50" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="28"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="45"/>
+    </row>
+    <row r="51" spans="1:5" s="4" customFormat="1">
+      <c r="A51" s="46"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="30"/>
+    </row>
+    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A52" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="28"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="72"/>
+      <c r="E54" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="9" t="s">
+    </row>
+    <row r="55" spans="1:5" s="42" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="49" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A46" s="46" t="s">
+      <c r="D55" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="48"/>
-    </row>
-    <row r="47" spans="1:5" s="4" customFormat="1">
-      <c r="A47" s="49"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="30"/>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A48" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="16"/>
-    </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A50" s="37"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="74" t="s">
+      <c r="E55" s="45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A56" s="54"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="E56" s="67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="12"/>
+    </row>
+    <row r="61" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="74"/>
-      <c r="E50" s="9" t="s">
+      <c r="D61" s="72"/>
+      <c r="E61" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A51" s="51"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="52" t="s">
+    <row r="62" spans="1:5" s="42" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A62" s="48"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D51" s="47" t="s">
+      <c r="D62" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="48" t="s">
+      <c r="E62" s="45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="12"/>
+    </row>
+    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="16"/>
+    </row>
+    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="72"/>
+      <c r="E66" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A67" s="48"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="16"/>
+    </row>
+    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:8" s="50" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="16"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+    </row>
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" s="72"/>
+      <c r="E72" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="12"/>
+    </row>
+    <row r="76" spans="1:8" s="50" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="16"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="51"/>
+    </row>
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A77" s="34"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77" s="72"/>
+      <c r="E77" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G77" s="52"/>
+    </row>
+    <row r="78" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A78" s="17"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="52"/>
+    </row>
+    <row r="79" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G79" s="52"/>
+    </row>
+    <row r="80" spans="1:8" s="4" customFormat="1" ht="13">
+      <c r="A80" s="17"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G80" s="52"/>
+    </row>
+    <row r="81" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G81" s="52"/>
+    </row>
+    <row r="82" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="72" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A52" s="57"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="73" t="s">
-        <v>162</v>
-      </c>
-      <c r="D52" s="69" t="s">
-        <v>163</v>
-      </c>
-      <c r="E52" s="70" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="16"/>
-    </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A55" s="21"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="16"/>
-    </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A57" s="37"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57" s="74"/>
-      <c r="E57" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="45" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A58" s="51"/>
-      <c r="B58" s="51"/>
-      <c r="C58" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" s="48" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="12"/>
-    </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="16"/>
-    </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="12"/>
-    </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
-      <c r="A62" s="37"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="D62" s="74"/>
-      <c r="E62" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A63" s="51"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="D63" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="E63" s="62" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="32"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="12"/>
-    </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A65" s="21"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A67" s="21"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="16"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="54"/>
-    </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="16"/>
-    </row>
-    <row r="71" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="12"/>
-    </row>
-    <row r="72" spans="1:8" s="53" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A72" s="21"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="16"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-    </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="74" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73" s="74"/>
-      <c r="E73" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G73" s="55"/>
-    </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G74" s="55"/>
-    </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A75" s="21"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G75" s="55"/>
-    </row>
-    <row r="76" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D76" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G76" s="55"/>
-    </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13">
-      <c r="A77" s="21"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="28" t="s">
+      <c r="D82" s="72"/>
+      <c r="E82" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D77" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G77" s="55"/>
-    </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="D78" s="74"/>
-      <c r="E78" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G78" s="55"/>
-    </row>
-    <row r="79" spans="1:8" s="4" customFormat="1" ht="25.5">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="D79" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="53" customFormat="1" ht="25.5">
-      <c r="A80" s="21"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="D80" s="65" t="s">
-        <v>139</v>
-      </c>
-      <c r="E80" s="62" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" ht="13">
-      <c r="A81" s="57"/>
-      <c r="B81" s="57"/>
-      <c r="C81" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="D81" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="E81" s="32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" ht="13">
-      <c r="A82" s="21"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D82" s="65" t="s">
-        <v>101</v>
-      </c>
-      <c r="E82" s="62" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" ht="25">
-      <c r="A83" s="42"/>
-      <c r="B83" s="42"/>
-      <c r="C83" s="32" t="s">
-        <v>123</v>
+      <c r="G82" s="52"/>
+    </row>
+    <row r="83" spans="1:7" s="4" customFormat="1" ht="25.5">
+      <c r="A83" s="17"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="E83" s="64" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="25.5">
+        <v>131</v>
+      </c>
+      <c r="E83" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="50" customFormat="1" ht="25.5">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
-      <c r="C84" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="D84" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="E84" s="62" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="72" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A85" s="57"/>
-      <c r="B85" s="57"/>
-      <c r="C85" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="D85" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="E85" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="F85" s="71"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="C84" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="E84" s="59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A85" s="54"/>
+      <c r="B85" s="54"/>
+      <c r="C85" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
-      <c r="C86" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="D86" s="65" t="s">
-        <v>142</v>
-      </c>
-      <c r="E86" s="62" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
-      <c r="A87" s="5"/>
-      <c r="B87" s="17"/>
+      <c r="C86" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="E86" s="59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="4" customFormat="1" ht="25">
+      <c r="A87" s="39"/>
+      <c r="B87" s="39"/>
       <c r="C87" s="32" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="E87" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="F87" s="55"/>
-    </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" ht="13">
+        <v>117</v>
+      </c>
+      <c r="E87" s="61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="4" customFormat="1" ht="25.5">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
-      <c r="C88" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="D88" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="E88" s="62" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A89" s="5"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="D89" s="33" t="s">
+      <c r="C88" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="D88" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="E88" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="69" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A89" s="54"/>
+      <c r="B89" s="54"/>
+      <c r="C89" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="D89" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="E89" s="67" t="s">
         <v>177</v>
       </c>
-      <c r="E89" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="F89" s="55"/>
-    </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" ht="13">
+      <c r="F89" s="68"/>
+    </row>
+    <row r="90" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
-      <c r="C90" s="63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D90" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="E90" s="62" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="C90" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D90" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="E90" s="59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
       <c r="C91" s="32" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="E91" s="64" t="s">
-        <v>202</v>
-      </c>
-      <c r="F91" s="55"/>
-    </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="13">
+        <v>136</v>
+      </c>
+      <c r="E91" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="F91" s="52"/>
+    </row>
+    <row r="92" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
-      <c r="C92" s="63" t="s">
-        <v>196</v>
-      </c>
-      <c r="D92" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="E92" s="62" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="C92" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="E92" s="59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="17"/>
       <c r="C93" s="32" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="E93" s="64" t="s">
-        <v>201</v>
-      </c>
-      <c r="F93" s="55"/>
-    </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" ht="13">
+        <v>168</v>
+      </c>
+      <c r="E93" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="F93" s="52"/>
+    </row>
+    <row r="94" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
-      <c r="C94" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D94" s="65" t="s">
-        <v>205</v>
-      </c>
-      <c r="E94" s="62" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="C94" s="60" t="s">
+        <v>171</v>
+      </c>
+      <c r="D94" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E94" s="59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A95" s="5"/>
       <c r="B95" s="17"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="31"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="55"/>
-    </row>
-    <row r="96" spans="1:6" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="C95" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D95" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E95" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="F95" s="52"/>
+    </row>
+    <row r="96" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A96" s="21"/>
       <c r="B96" s="21"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="29"/>
-      <c r="E96" s="16"/>
+      <c r="C96" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="E96" s="59" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="17"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="31"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="55"/>
+      <c r="C97" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D97" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E97" s="61" t="s">
+        <v>192</v>
+      </c>
+      <c r="F97" s="52"/>
     </row>
     <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="16"/>
-    </row>
-    <row r="99" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
-      <c r="A99" s="37"/>
-      <c r="B99" s="37"/>
-      <c r="C99" s="74" t="s">
+      <c r="C98" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="D98" s="62" t="s">
+        <v>196</v>
+      </c>
+      <c r="E98" s="59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A99" s="5"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="31"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="52"/>
+    </row>
+    <row r="100" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A100" s="21"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="16"/>
+    </row>
+    <row r="101" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
+      <c r="A101" s="5"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="52"/>
+    </row>
+    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A102" s="21"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="16"/>
+    </row>
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+      <c r="A103" s="34"/>
+      <c r="B103" s="34"/>
+      <c r="C103" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D103" s="72"/>
+      <c r="E103" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G103" s="52"/>
+    </row>
+    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D104" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E104" s="38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A105" s="21"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="29"/>
+      <c r="E105" s="16"/>
+    </row>
+    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+      <c r="A106" s="34"/>
+      <c r="B106" s="34"/>
+      <c r="C106" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" s="55"/>
+      <c r="E106" s="35" t="s">
         <v>55</v>
-      </c>
-      <c r="D99" s="74"/>
-      <c r="E99" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G99" s="55"/>
-    </row>
-    <row r="100" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="E100" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A101" s="21"/>
-      <c r="B101" s="21"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="16"/>
-    </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A102" s="37"/>
-      <c r="B102" s="37"/>
-      <c r="C102" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D102" s="58"/>
-      <c r="E102" s="38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D103" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="E103" s="64" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A104" s="21"/>
-      <c r="B104" s="21"/>
-      <c r="C104" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D104" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E104" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D105" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="E105" s="59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
-      <c r="A106" s="21"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D106" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E106" s="60" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="E107" s="64" t="s">
-        <v>31</v>
+        <v>156</v>
+      </c>
+      <c r="E107" s="61" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
-      <c r="C108" s="28" t="s">
-        <v>69</v>
+      <c r="C108" s="60" t="s">
+        <v>219</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
-      <c r="C109" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D109" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E109" s="20" t="s">
-        <v>72</v>
+      <c r="C109" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D109" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E109" s="56" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>74</v>
+        <v>62</v>
+      </c>
+      <c r="E110" s="57" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
-      <c r="C111" s="30" t="s">
-        <v>75</v>
+      <c r="C111" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="E111" s="30" t="s">
-        <v>31</v>
+        <v>151</v>
+      </c>
+      <c r="E111" s="61" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D113" s="31" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E113" s="20" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
-      <c r="C114" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="D114" s="65" t="s">
-        <v>173</v>
-      </c>
-      <c r="E114" s="62" t="s">
-        <v>31</v>
+      <c r="C114" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D114" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E114" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="32" t="s">
-        <v>172</v>
+      <c r="A115" s="5"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="E115" s="64" t="s">
-        <v>31</v>
+        <v>157</v>
+      </c>
+      <c r="E115" s="30" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
-      <c r="C116" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="D116" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="E116" s="62" t="s">
-        <v>31</v>
+      <c r="C116" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="D117" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="E117" s="64" t="s">
-        <v>31</v>
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="D117" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="E117" s="67" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="29"/>
-      <c r="E118" s="16"/>
+      <c r="C118" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="D118" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="E118" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
-      <c r="C119" s="41"/>
-      <c r="D119" s="42"/>
-      <c r="E119" s="20"/>
+      <c r="C119" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D119" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="E119" s="61" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="29"/>
-      <c r="E120" s="16"/>
+      <c r="C120" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="D120" s="62" t="s">
+        <v>176</v>
+      </c>
+      <c r="E120" s="59" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
-      <c r="C121" s="41"/>
-      <c r="D121" s="42"/>
-      <c r="E121" s="20"/>
+      <c r="C121" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D121" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E121" s="61" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A122" s="21"/>
@@ -2740,8 +2800,8 @@
     <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
-      <c r="C123" s="41"/>
-      <c r="D123" s="42"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="39"/>
       <c r="E123" s="20"/>
     </row>
     <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
@@ -2754,8 +2814,8 @@
     <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
-      <c r="C125" s="41"/>
-      <c r="D125" s="42"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="39"/>
       <c r="E125" s="20"/>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
@@ -2768,8 +2828,8 @@
     <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
-      <c r="C127" s="41"/>
-      <c r="D127" s="42"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="39"/>
       <c r="E127" s="20"/>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
@@ -2780,618 +2840,618 @@
       <c r="E128" s="16"/>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
-      <c r="A129" s="5"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D129" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E129" s="30" t="s">
-        <v>31</v>
-      </c>
+      <c r="A129" s="17"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="38"/>
+      <c r="D129" s="39"/>
+      <c r="E129" s="20"/>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
-      <c r="C130" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D130" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E130" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" s="4" customFormat="1">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="61"/>
-    </row>
-    <row r="132" spans="1:5" s="4" customFormat="1">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="61"/>
-    </row>
-    <row r="133" spans="1:5" s="4" customFormat="1">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="61"/>
-    </row>
-    <row r="134" spans="1:5" s="4" customFormat="1">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="61"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="29"/>
+      <c r="E130" s="16"/>
+    </row>
+    <row r="131" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A131" s="17"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="38"/>
+      <c r="D131" s="39"/>
+      <c r="E131" s="20"/>
+    </row>
+    <row r="132" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A132" s="21"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="28"/>
+      <c r="D132" s="29"/>
+      <c r="E132" s="16"/>
+    </row>
+    <row r="133" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D133" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E133" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="A134" s="21"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D134" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E134" s="16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
-      <c r="E135" s="61"/>
+      <c r="E135" s="58"/>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="2"/>
-      <c r="E136" s="61"/>
+      <c r="E136" s="58"/>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="61"/>
+      <c r="E137" s="58"/>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="2"/>
-      <c r="E138" s="61"/>
+      <c r="E138" s="58"/>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
-      <c r="E139" s="61"/>
+      <c r="E139" s="58"/>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="2"/>
-      <c r="E140" s="61"/>
+      <c r="E140" s="58"/>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
-      <c r="E141" s="61"/>
+      <c r="E141" s="58"/>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
-      <c r="E142" s="61"/>
+      <c r="E142" s="58"/>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="61"/>
+      <c r="E143" s="58"/>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="2"/>
-      <c r="E144" s="61"/>
+      <c r="E144" s="58"/>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="2"/>
-      <c r="E145" s="61"/>
+      <c r="E145" s="58"/>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
-      <c r="E146" s="61"/>
+      <c r="E146" s="58"/>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
-      <c r="E147" s="61"/>
+      <c r="E147" s="58"/>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
-      <c r="E148" s="61"/>
+      <c r="E148" s="58"/>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="2"/>
-      <c r="E149" s="61"/>
+      <c r="E149" s="58"/>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="2"/>
-      <c r="E150" s="61"/>
+      <c r="E150" s="58"/>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="2"/>
-      <c r="E151" s="61"/>
+      <c r="E151" s="58"/>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="61"/>
+      <c r="E152" s="58"/>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
-      <c r="E153" s="61"/>
+      <c r="E153" s="58"/>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="2"/>
-      <c r="E154" s="61"/>
+      <c r="E154" s="58"/>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="2"/>
-      <c r="E155" s="61"/>
+      <c r="E155" s="58"/>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="2"/>
-      <c r="E156" s="61"/>
+      <c r="E156" s="58"/>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="2"/>
-      <c r="E157" s="61"/>
+      <c r="E157" s="58"/>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="61"/>
+      <c r="E158" s="58"/>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="2"/>
-      <c r="E159" s="61"/>
+      <c r="E159" s="58"/>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="61"/>
+      <c r="E160" s="58"/>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="2"/>
-      <c r="E161" s="61"/>
+      <c r="E161" s="58"/>
     </row>
     <row r="162" spans="1:5" s="4" customFormat="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="61"/>
+      <c r="E162" s="58"/>
     </row>
     <row r="163" spans="1:5" s="4" customFormat="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
-      <c r="E163" s="61"/>
+      <c r="E163" s="58"/>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="2"/>
-      <c r="E164" s="61"/>
+      <c r="E164" s="58"/>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="2"/>
-      <c r="E165" s="61"/>
+      <c r="E165" s="58"/>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="2"/>
-      <c r="E166" s="61"/>
+      <c r="E166" s="58"/>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="2"/>
-      <c r="E167" s="61"/>
+      <c r="E167" s="58"/>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="2"/>
-      <c r="E168" s="61"/>
+      <c r="E168" s="58"/>
     </row>
     <row r="169" spans="1:5" s="4" customFormat="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="2"/>
-      <c r="E169" s="61"/>
+      <c r="E169" s="58"/>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="2"/>
-      <c r="E170" s="61"/>
+      <c r="E170" s="58"/>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="2"/>
-      <c r="E171" s="61"/>
+      <c r="E171" s="58"/>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="2"/>
-      <c r="E172" s="61"/>
+      <c r="E172" s="58"/>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="2"/>
-      <c r="E173" s="61"/>
+      <c r="E173" s="58"/>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="2"/>
-      <c r="E174" s="61"/>
+      <c r="E174" s="58"/>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="2"/>
-      <c r="E175" s="61"/>
+      <c r="E175" s="58"/>
     </row>
     <row r="176" spans="1:5" s="4" customFormat="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
-      <c r="E176" s="61"/>
+      <c r="E176" s="58"/>
     </row>
     <row r="177" spans="1:5" s="4" customFormat="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="2"/>
-      <c r="E177" s="61"/>
+      <c r="E177" s="58"/>
     </row>
     <row r="178" spans="1:5" s="4" customFormat="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="2"/>
-      <c r="E178" s="61"/>
+      <c r="E178" s="58"/>
     </row>
     <row r="179" spans="1:5" s="4" customFormat="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="2"/>
-      <c r="E179" s="61"/>
+      <c r="E179" s="58"/>
     </row>
     <row r="180" spans="1:5" s="4" customFormat="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="2"/>
-      <c r="E180" s="61"/>
+      <c r="E180" s="58"/>
     </row>
     <row r="181" spans="1:5" s="4" customFormat="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="2"/>
-      <c r="E181" s="61"/>
+      <c r="E181" s="58"/>
     </row>
     <row r="182" spans="1:5" s="4" customFormat="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="2"/>
-      <c r="E182" s="61"/>
+      <c r="E182" s="58"/>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="2"/>
-      <c r="E183" s="61"/>
+      <c r="E183" s="58"/>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="2"/>
-      <c r="E184" s="61"/>
+      <c r="E184" s="58"/>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="2"/>
-      <c r="E185" s="61"/>
+      <c r="E185" s="58"/>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="2"/>
-      <c r="E186" s="61"/>
+      <c r="E186" s="58"/>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="2"/>
-      <c r="E187" s="61"/>
+      <c r="E187" s="58"/>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="2"/>
-      <c r="E188" s="61"/>
+      <c r="E188" s="58"/>
     </row>
     <row r="189" spans="1:5" s="4" customFormat="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="2"/>
-      <c r="E189" s="61"/>
+      <c r="E189" s="58"/>
     </row>
     <row r="190" spans="1:5" s="4" customFormat="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="2"/>
-      <c r="E190" s="61"/>
+      <c r="E190" s="58"/>
     </row>
     <row r="191" spans="1:5" s="4" customFormat="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="2"/>
-      <c r="E191" s="61"/>
+      <c r="E191" s="58"/>
     </row>
     <row r="192" spans="1:5" s="4" customFormat="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="2"/>
-      <c r="E192" s="61"/>
+      <c r="E192" s="58"/>
     </row>
     <row r="193" spans="1:5" s="4" customFormat="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="2"/>
-      <c r="E193" s="61"/>
+      <c r="E193" s="58"/>
     </row>
     <row r="194" spans="1:5" s="4" customFormat="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="2"/>
-      <c r="E194" s="61"/>
+      <c r="E194" s="58"/>
     </row>
     <row r="195" spans="1:5" s="4" customFormat="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="2"/>
-      <c r="E195" s="61"/>
+      <c r="E195" s="58"/>
     </row>
     <row r="196" spans="1:5" s="4" customFormat="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="2"/>
-      <c r="E196" s="61"/>
+      <c r="E196" s="58"/>
     </row>
     <row r="197" spans="1:5" s="4" customFormat="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="2"/>
-      <c r="E197" s="61"/>
+      <c r="E197" s="58"/>
     </row>
     <row r="198" spans="1:5" s="4" customFormat="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="2"/>
-      <c r="E198" s="61"/>
+      <c r="E198" s="58"/>
     </row>
     <row r="199" spans="1:5" s="4" customFormat="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="2"/>
-      <c r="E199" s="61"/>
+      <c r="E199" s="58"/>
     </row>
     <row r="200" spans="1:5" s="4" customFormat="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="2"/>
-      <c r="E200" s="61"/>
+      <c r="E200" s="58"/>
     </row>
     <row r="201" spans="1:5" s="4" customFormat="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="2"/>
-      <c r="E201" s="61"/>
+      <c r="E201" s="58"/>
     </row>
     <row r="202" spans="1:5" s="4" customFormat="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="2"/>
-      <c r="E202" s="61"/>
+      <c r="E202" s="58"/>
     </row>
     <row r="203" spans="1:5" s="4" customFormat="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="2"/>
-      <c r="E203" s="61"/>
+      <c r="E203" s="58"/>
     </row>
     <row r="204" spans="1:5" s="4" customFormat="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="2"/>
-      <c r="E204" s="61"/>
+      <c r="E204" s="58"/>
     </row>
     <row r="205" spans="1:5" s="4" customFormat="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="2"/>
-      <c r="E205" s="61"/>
+      <c r="E205" s="58"/>
     </row>
     <row r="206" spans="1:5" s="4" customFormat="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="2"/>
-      <c r="E206" s="61"/>
+      <c r="E206" s="58"/>
     </row>
     <row r="207" spans="1:5" s="4" customFormat="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="2"/>
-      <c r="E207" s="61"/>
+      <c r="E207" s="58"/>
     </row>
     <row r="208" spans="1:5" s="4" customFormat="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="2"/>
-      <c r="E208" s="61"/>
+      <c r="E208" s="58"/>
     </row>
     <row r="209" spans="1:5" s="4" customFormat="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="2"/>
-      <c r="E209" s="61"/>
+      <c r="E209" s="58"/>
     </row>
     <row r="210" spans="1:5" s="4" customFormat="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="2"/>
-      <c r="E210" s="61"/>
+      <c r="E210" s="58"/>
     </row>
     <row r="211" spans="1:5" s="4" customFormat="1">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="2"/>
-      <c r="E211" s="3"/>
+      <c r="E211" s="58"/>
     </row>
     <row r="212" spans="1:5" s="4" customFormat="1">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="2"/>
-      <c r="E212" s="3"/>
+      <c r="E212" s="58"/>
     </row>
     <row r="213" spans="1:5" s="4" customFormat="1">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="2"/>
-      <c r="E213" s="3"/>
+      <c r="E213" s="58"/>
     </row>
     <row r="214" spans="1:5" s="4" customFormat="1">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="2"/>
-      <c r="E214" s="3"/>
+      <c r="E214" s="58"/>
     </row>
     <row r="215" spans="1:5" s="4" customFormat="1">
       <c r="A215" s="1"/>
@@ -3680,20 +3740,48 @@
       <c r="D255" s="2"/>
       <c r="E255" s="3"/>
     </row>
+    <row r="256" spans="1:5" s="4" customFormat="1">
+      <c r="A256" s="1"/>
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
+      <c r="D256" s="2"/>
+      <c r="E256" s="3"/>
+    </row>
+    <row r="257" spans="1:5" s="4" customFormat="1">
+      <c r="A257" s="1"/>
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
+      <c r="D257" s="2"/>
+      <c r="E257" s="3"/>
+    </row>
+    <row r="258" spans="1:5" s="4" customFormat="1">
+      <c r="A258" s="1"/>
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+      <c r="D258" s="2"/>
+      <c r="E258" s="3"/>
+    </row>
+    <row r="259" spans="1:5" s="4" customFormat="1">
+      <c r="A259" s="1"/>
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C77:D77"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed climb motor port in current year and changed values in auto
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 2022.xlsx
+++ b/Kilroy Equipment List 2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$105</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="226">
   <si>
     <t>Code Written/Tested</t>
   </si>
@@ -360,9 +360,6 @@
     <t>DIO 24</t>
   </si>
   <si>
-    <t>DIO 23</t>
-  </si>
-  <si>
     <t>DIO 22</t>
   </si>
   <si>
@@ -682,6 +679,27 @@
   </si>
   <si>
     <t>Classmate/Toshiba DriverStation</t>
+  </si>
+  <si>
+    <t>Demo switch</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Channel 2</t>
+  </si>
+  <si>
+    <t>rightOperatorThrottleValue</t>
+  </si>
+  <si>
+    <t>Right Operator Throttle</t>
+  </si>
+  <si>
+    <t>DIO 25</t>
   </si>
 </sst>
 </file>
@@ -1073,17 +1091,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,7 +1409,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1402,33 +1420,33 @@
   <dimension ref="A1:AMK259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C117" sqref="C117:E117"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" style="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="26">
+      <c r="A1" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1463,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="61" t="s">
         <v>99</v>
@@ -1476,7 +1494,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="59" t="s">
         <v>98</v>
@@ -1489,97 +1507,97 @@
         <v>9</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="22" customFormat="1" ht="13">
+    <row r="7" spans="1:8" s="22" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="59" t="s">
         <v>142</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>143</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -1589,16 +1607,16 @@
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="13">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="32" t="s">
@@ -1611,7 +1629,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="60" t="s">
@@ -1624,7 +1642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="32" t="s">
@@ -1637,20 +1655,20 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="E17" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="32" t="s">
@@ -1663,64 +1681,64 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="19" spans="1:8" s="4" customFormat="1">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="E19" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="59" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20" s="71" t="s">
         <v>210</v>
       </c>
-      <c r="D20" s="74" t="s">
+      <c r="E20" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="E20" s="63" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="60" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="E21" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="E21" s="59" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="47"/>
-      <c r="D22" s="74"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="63"/>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A23" s="34"/>
       <c r="B23" s="34"/>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="73"/>
+      <c r="D23" s="74"/>
       <c r="E23" s="35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="24" spans="1:8" s="4" customFormat="1">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="60" t="s">
@@ -1730,10 +1748,10 @@
         <v>107</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="13">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="32" t="s">
@@ -1743,10 +1761,10 @@
         <v>108</v>
       </c>
       <c r="E25" s="61" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="60" t="s">
@@ -1756,13 +1774,13 @@
         <v>109</v>
       </c>
       <c r="E26" s="59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="27" spans="1:8" s="4" customFormat="1">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="C27" s="32" t="s">
@@ -1772,13 +1790,13 @@
         <v>110</v>
       </c>
       <c r="E27" s="61" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="28" spans="1:8" s="4" customFormat="1">
       <c r="A28" s="37"/>
       <c r="B28" s="37"/>
       <c r="C28" s="60"/>
@@ -1788,7 +1806,7 @@
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="C29" s="32"/>
@@ -1798,7 +1816,7 @@
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="28"/>
@@ -1808,7 +1826,7 @@
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="31" spans="1:8" s="4" customFormat="1">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="38"/>
@@ -1818,7 +1836,7 @@
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
       <c r="C32" s="72" t="s">
@@ -1829,7 +1847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="37"/>
       <c r="B33" s="37"/>
       <c r="C33" s="28" t="s">
@@ -1842,7 +1860,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="30" t="s">
@@ -1855,88 +1873,94 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D36" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E36" s="61" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="D37" s="62" t="s">
+      <c r="E37" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="59" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="13">
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="20"/>
-    </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="13">
+      <c r="C38" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="28"/>
       <c r="D39" s="40"/>
       <c r="E39" s="16"/>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="40" spans="1:5" s="4" customFormat="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
       <c r="E40" s="20"/>
     </row>
-    <row r="41" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="41" spans="1:5" s="4" customFormat="1">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="42" spans="1:5" s="4" customFormat="1">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
       <c r="C42" s="32"/>
       <c r="D42" s="41"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="43" spans="1:5" s="4" customFormat="1">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="28"/>
       <c r="D43" s="29"/>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="1:5" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="44" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="30"/>
@@ -1982,7 +2006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="50" spans="1:5" s="4" customFormat="1">
       <c r="A50" s="43" t="s">
         <v>21</v>
       </c>
@@ -2000,7 +2024,7 @@
       <c r="D51" s="31"/>
       <c r="E51" s="30"/>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="52" spans="1:5" s="4" customFormat="1">
       <c r="A52" s="21" t="s">
         <v>21</v>
       </c>
@@ -2011,7 +2035,7 @@
       <c r="D52" s="29"/>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="53" spans="1:5" s="4" customFormat="1">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="38"/>
@@ -2042,41 +2066,41 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="56" spans="1:5" s="4" customFormat="1">
       <c r="A56" s="54"/>
       <c r="B56" s="54"/>
       <c r="C56" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="66" t="s">
         <v>153</v>
-      </c>
-      <c r="D56" s="66" t="s">
-        <v>154</v>
       </c>
       <c r="E56" s="67" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="57" spans="1:5" s="4" customFormat="1">
       <c r="A57" s="21"/>
       <c r="B57" s="21"/>
       <c r="C57" s="28"/>
       <c r="D57" s="29"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="58" spans="1:5" s="4" customFormat="1">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="32"/>
       <c r="D58" s="33"/>
       <c r="E58" s="12"/>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="59" spans="1:5" s="4" customFormat="1">
       <c r="A59" s="21"/>
       <c r="B59" s="21"/>
       <c r="C59" s="28"/>
       <c r="D59" s="29"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="60" spans="1:5" s="4" customFormat="1">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
       <c r="C60" s="32"/>
@@ -2107,28 +2131,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="63" spans="1:5" s="4" customFormat="1">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="38"/>
       <c r="D63" s="33"/>
       <c r="E63" s="12"/>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="64" spans="1:5" s="4" customFormat="1">
       <c r="A64" s="21"/>
       <c r="B64" s="21"/>
       <c r="C64" s="28"/>
       <c r="D64" s="29"/>
       <c r="E64" s="16"/>
     </row>
-    <row r="65" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="65" spans="1:8" s="4" customFormat="1">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="C65" s="32"/>
       <c r="D65" s="33"/>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="66" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A66" s="34"/>
       <c r="B66" s="34"/>
       <c r="C66" s="72" t="s">
@@ -2139,34 +2163,34 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="67" spans="1:8" s="4" customFormat="1">
       <c r="A67" s="48"/>
       <c r="B67" s="48"/>
       <c r="C67" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E67" s="59" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" s="4" customFormat="1" ht="13">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="4" customFormat="1">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="32"/>
       <c r="D68" s="33"/>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="21"/>
       <c r="B69" s="21"/>
       <c r="C69" s="28"/>
       <c r="D69" s="29"/>
       <c r="E69" s="16"/>
     </row>
-    <row r="70" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="70" spans="1:8" s="4" customFormat="1">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="32"/>
@@ -2182,7 +2206,7 @@
       <c r="G71" s="51"/>
       <c r="H71" s="51"/>
     </row>
-    <row r="72" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="72" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A72" s="34"/>
       <c r="B72" s="34"/>
       <c r="C72" s="72" t="s">
@@ -2193,7 +2217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="73" spans="1:8" s="4" customFormat="1">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="38" t="s">
@@ -2206,14 +2230,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="74" spans="1:8" s="4" customFormat="1">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="28"/>
       <c r="D74" s="29"/>
       <c r="E74" s="16"/>
     </row>
-    <row r="75" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="75" spans="1:8" s="4" customFormat="1">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="38"/>
@@ -2229,7 +2253,7 @@
       <c r="G76" s="51"/>
       <c r="H76" s="51"/>
     </row>
-    <row r="77" spans="1:8" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="77" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A77" s="34"/>
       <c r="B77" s="34"/>
       <c r="C77" s="72" t="s">
@@ -2241,7 +2265,7 @@
       </c>
       <c r="G77" s="52"/>
     </row>
-    <row r="78" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="78" spans="1:8" s="4" customFormat="1">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="32" t="s">
@@ -2255,7 +2279,7 @@
       </c>
       <c r="G78" s="52"/>
     </row>
-    <row r="79" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="79" spans="1:8" s="4" customFormat="1">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="28" t="s">
@@ -2269,7 +2293,7 @@
       </c>
       <c r="G79" s="52"/>
     </row>
-    <row r="80" spans="1:8" s="4" customFormat="1" ht="13">
+    <row r="80" spans="1:8" s="4" customFormat="1">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="30" t="s">
@@ -2283,7 +2307,7 @@
       </c>
       <c r="G80" s="52"/>
     </row>
-    <row r="81" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="81" spans="1:7" s="4" customFormat="1">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="28" t="s">
@@ -2297,7 +2321,7 @@
       </c>
       <c r="G81" s="52"/>
     </row>
-    <row r="82" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="82" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A82" s="34"/>
       <c r="B82" s="34"/>
       <c r="C82" s="72" t="s">
@@ -2316,10 +2340,10 @@
         <v>81</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="50" customFormat="1" ht="25.5">
@@ -2329,17 +2353,17 @@
         <v>82</v>
       </c>
       <c r="D84" s="62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E84" s="59" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="4" customFormat="1" ht="13">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="4" customFormat="1">
       <c r="A85" s="54"/>
       <c r="B85" s="54"/>
       <c r="C85" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D85" s="32" t="s">
         <v>95</v>
@@ -2348,7 +2372,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="86" spans="1:7" s="4" customFormat="1">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="59" t="s">
@@ -2361,173 +2385,179 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="4" customFormat="1" ht="25">
+    <row r="87" spans="1:7" s="4" customFormat="1" ht="25.5">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D87" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D87" s="33" t="s">
+      <c r="E87" s="61" t="s">
         <v>117</v>
-      </c>
-      <c r="E87" s="61" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:7" s="4" customFormat="1" ht="25.5">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D88" s="62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E88" s="59" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="69" customFormat="1" ht="13.15" customHeight="1">
       <c r="A89" s="54"/>
       <c r="B89" s="54"/>
       <c r="C89" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D89" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E89" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F89" s="68"/>
     </row>
-    <row r="90" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="90" spans="1:7" s="4" customFormat="1">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D90" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E90" s="59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A91" s="5"/>
       <c r="B91" s="17"/>
       <c r="C91" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E91" s="61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F91" s="52"/>
     </row>
-    <row r="92" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="92" spans="1:7" s="4" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D92" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="E92" s="59" t="s">
         <v>166</v>
-      </c>
-      <c r="E92" s="59" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A93" s="5"/>
       <c r="B93" s="17"/>
       <c r="C93" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E93" s="53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F93" s="52"/>
     </row>
-    <row r="94" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="94" spans="1:7" s="4" customFormat="1">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D94" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="D94" s="62" t="s">
+      <c r="E94" s="59" t="s">
         <v>172</v>
-      </c>
-      <c r="E94" s="59" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A95" s="5"/>
       <c r="B95" s="17"/>
       <c r="C95" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="D95" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="D95" s="33" t="s">
-        <v>185</v>
-      </c>
       <c r="E95" s="61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F95" s="52"/>
     </row>
-    <row r="96" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="96" spans="1:7" s="4" customFormat="1">
       <c r="A96" s="21"/>
       <c r="B96" s="21"/>
       <c r="C96" s="60" t="s">
+        <v>186</v>
+      </c>
+      <c r="D96" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="D96" s="62" t="s">
-        <v>188</v>
-      </c>
       <c r="E96" s="59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="17"/>
       <c r="C97" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D97" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="D97" s="33" t="s">
+      <c r="E97" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="E97" s="61" t="s">
-        <v>192</v>
-      </c>
       <c r="F97" s="52"/>
     </row>
-    <row r="98" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="98" spans="1:7" s="4" customFormat="1">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="D98" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="D98" s="62" t="s">
-        <v>196</v>
-      </c>
       <c r="E98" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A99" s="5"/>
       <c r="B99" s="17"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="31"/>
-      <c r="E99" s="20"/>
+      <c r="C99" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D99" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="E99" s="61" t="s">
+        <v>222</v>
+      </c>
       <c r="F99" s="52"/>
     </row>
     <row r="100" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1">
@@ -2545,14 +2575,14 @@
       <c r="E101" s="20"/>
       <c r="F101" s="52"/>
     </row>
-    <row r="102" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="102" spans="1:7" s="4" customFormat="1">
       <c r="A102" s="21"/>
       <c r="B102" s="21"/>
       <c r="C102" s="28"/>
       <c r="D102" s="29"/>
       <c r="E102" s="16"/>
     </row>
-    <row r="103" spans="1:7" s="4" customFormat="1" ht="13.4" customHeight="1">
+    <row r="103" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A103" s="34"/>
       <c r="B103" s="34"/>
       <c r="C103" s="72" t="s">
@@ -2564,7 +2594,7 @@
       </c>
       <c r="G103" s="52"/>
     </row>
-    <row r="104" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="104" spans="1:7" s="4" customFormat="1">
       <c r="A104" s="17"/>
       <c r="B104" s="17"/>
       <c r="C104" s="53" t="s">
@@ -2577,14 +2607,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="21"/>
       <c r="B105" s="21"/>
       <c r="C105" s="28"/>
       <c r="D105" s="29"/>
       <c r="E105" s="16"/>
     </row>
-    <row r="106" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="34"/>
       <c r="B106" s="34"/>
       <c r="C106" s="35" t="s">
@@ -2595,24 +2625,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="107" spans="1:7" s="4" customFormat="1">
       <c r="A107" s="5"/>
       <c r="B107" s="5"/>
       <c r="C107" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D107" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="D107" s="33" t="s">
-        <v>156</v>
-      </c>
       <c r="E107" s="61" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="4" customFormat="1" ht="13">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="4" customFormat="1">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D108" s="29" t="s">
         <v>56</v>
@@ -2621,7 +2651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="38" t="s">
@@ -2634,7 +2664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="28" t="s">
@@ -2647,20 +2677,20 @@
         <v>63</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E111" s="61" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="4" customFormat="1" ht="13">
+    <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="28" t="s">
@@ -2673,7 +2703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="30" t="s">
@@ -2686,7 +2716,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="28" t="s">
@@ -2699,20 +2729,20 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="115" spans="1:5" s="4" customFormat="1">
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="30" t="s">
         <v>70</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E115" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="28" t="s">
@@ -2725,7 +2755,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
       <c r="C117" s="70" t="s">
@@ -2738,136 +2768,136 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
       <c r="C118" s="60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D118" s="62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E118" s="59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="119" spans="1:5" s="4" customFormat="1">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D119" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E119" s="61" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="120" spans="1:5" s="4" customFormat="1">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
       <c r="C120" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="D120" s="62" t="s">
         <v>175</v>
-      </c>
-      <c r="D120" s="62" t="s">
-        <v>176</v>
       </c>
       <c r="E120" s="59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="D121" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="D121" s="33" t="s">
-        <v>183</v>
       </c>
       <c r="E121" s="61" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="21"/>
       <c r="B122" s="21"/>
       <c r="C122" s="28"/>
       <c r="D122" s="29"/>
       <c r="E122" s="16"/>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="38"/>
       <c r="D123" s="39"/>
       <c r="E123" s="20"/>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="124" spans="1:5" s="4" customFormat="1">
       <c r="A124" s="21"/>
       <c r="B124" s="21"/>
       <c r="C124" s="28"/>
       <c r="D124" s="29"/>
       <c r="E124" s="16"/>
     </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="125" spans="1:5" s="4" customFormat="1">
       <c r="A125" s="17"/>
       <c r="B125" s="17"/>
       <c r="C125" s="38"/>
       <c r="D125" s="39"/>
       <c r="E125" s="20"/>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="21"/>
       <c r="B126" s="21"/>
       <c r="C126" s="28"/>
       <c r="D126" s="29"/>
       <c r="E126" s="16"/>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="17"/>
       <c r="B127" s="17"/>
       <c r="C127" s="38"/>
       <c r="D127" s="39"/>
       <c r="E127" s="20"/>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="21"/>
       <c r="B128" s="21"/>
       <c r="C128" s="28"/>
       <c r="D128" s="29"/>
       <c r="E128" s="16"/>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="17"/>
       <c r="B129" s="17"/>
       <c r="C129" s="38"/>
       <c r="D129" s="39"/>
       <c r="E129" s="20"/>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
       <c r="C130" s="28"/>
       <c r="D130" s="29"/>
       <c r="E130" s="16"/>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="17"/>
       <c r="B131" s="17"/>
       <c r="C131" s="38"/>
       <c r="D131" s="39"/>
       <c r="E131" s="20"/>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="21"/>
       <c r="B132" s="21"/>
       <c r="C132" s="28"/>
       <c r="D132" s="29"/>
       <c r="E132" s="16"/>
     </row>
-    <row r="133" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="133" spans="1:5" s="4" customFormat="1">
       <c r="A133" s="5"/>
       <c r="B133" s="5"/>
       <c r="C133" s="30" t="s">
@@ -2880,7 +2910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" ht="13">
+    <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="21"/>
       <c r="B134" s="21"/>
       <c r="C134" s="28" t="s">
@@ -3770,6 +3800,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C54:D54"/>
@@ -3777,11 +3812,6 @@
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="C77:D77"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>